<commit_message>
test specs for leaderboard func started
</commit_message>
<xml_diff>
--- a/excel-docs/euro - lifecycle info.xlsx
+++ b/excel-docs/euro - lifecycle info.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joseph.collins/Documents/personal-projects/world cup/world-cup-OG/excel docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joseph.collins/Documents/personal-projects/euro/2024_euro/excel-docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73AF7875-694D-9C47-80FA-6313CCC90CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9196DE-BF60-0244-8F66-37138810B7F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20140" xr2:uid="{D89656BD-B983-D041-A997-C1184058734E}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20060" activeTab="3" xr2:uid="{D89656BD-B983-D041-A997-C1184058734E}"/>
   </bookViews>
   <sheets>
     <sheet name="life cycle actions" sheetId="6" r:id="rId1"/>
     <sheet name="part scenarios" sheetId="4" r:id="rId2"/>
     <sheet name="error testing" sheetId="3" r:id="rId3"/>
-    <sheet name="emails" sheetId="7" r:id="rId4"/>
+    <sheet name="tiebreaker testing scneari" sheetId="8" r:id="rId4"/>
+    <sheet name="emails" sheetId="7" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,8 +27,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="134">
   <si>
     <t>need to submit a number for tiebreaker score</t>
   </si>
@@ -461,12 +465,75 @@
   <si>
     <t>what does it look like for Test's login</t>
   </si>
+  <si>
+    <t>scenario #</t>
+  </si>
+  <si>
+    <t>winner</t>
+  </si>
+  <si>
+    <t>actual total goals</t>
+  </si>
+  <si>
+    <t>part 1 total goals</t>
+  </si>
+  <si>
+    <t>part 2 total goals</t>
+  </si>
+  <si>
+    <t>test written?</t>
+  </si>
+  <si>
+    <t>part 1 total is under, part 2 is over</t>
+  </si>
+  <si>
+    <t>part 1</t>
+  </si>
+  <si>
+    <t>part 2 total is under, part 1 is over</t>
+  </si>
+  <si>
+    <t>part 2</t>
+  </si>
+  <si>
+    <t>part 1 total is exact, part 2 total is under</t>
+  </si>
+  <si>
+    <t>part 2 total is exact, part 1 total is under</t>
+  </si>
+  <si>
+    <t>part 1 total is exact, part 2 total is over</t>
+  </si>
+  <si>
+    <t>part 2 total is exact, part 1 total is over</t>
+  </si>
+  <si>
+    <t>both totals are over the actual total</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>both totals are under the actual total</t>
+  </si>
+  <si>
+    <t>part 1 is closer to actual total</t>
+  </si>
+  <si>
+    <t>part 2 is closer to actual total</t>
+  </si>
+  <si>
+    <t>both parts have the same tiebreaker score</t>
+  </si>
+  <si>
+    <t>throw error</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -540,8 +607,23 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -578,8 +660,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8D9B"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00D200"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -657,11 +775,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -728,48 +870,121 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -793,7 +1008,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1081,7 +1296,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1094,7 +1309,7 @@
   </sheetPr>
   <dimension ref="A1:F105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="160" workbookViewId="0">
+    <sheetView topLeftCell="A47" zoomScale="160" workbookViewId="0">
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
@@ -1118,7 +1333,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="36">
+      <c r="A2" s="39">
         <v>1</v>
       </c>
       <c r="B2" s="32" t="s">
@@ -1126,19 +1341,19 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="36"/>
+      <c r="A3" s="39"/>
       <c r="B3" s="32" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="36"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="32" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="36"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="32" t="s">
         <v>16</v>
       </c>
@@ -1148,7 +1363,7 @@
       <c r="B6" s="15"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="38">
+      <c r="A7" s="41">
         <v>2</v>
       </c>
       <c r="B7" s="32" t="s">
@@ -1156,7 +1371,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="39"/>
+      <c r="A8" s="42"/>
       <c r="B8" s="33" t="s">
         <v>94</v>
       </c>
@@ -1166,7 +1381,7 @@
       <c r="B9" s="7"/>
     </row>
     <row r="10" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="37">
+      <c r="A10" s="40">
         <v>3</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -1174,79 +1389,79 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="24" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="37"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="23" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="24" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="37"/>
+      <c r="A12" s="40"/>
       <c r="B12" s="23" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="37"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="34" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="37"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="34" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="37"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="34" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="37"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="34" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="37"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="34" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="37"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="34" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="37"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="34" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="37"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="34" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="37"/>
+      <c r="A21" s="40"/>
       <c r="B21" s="34" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="37"/>
+      <c r="A22" s="40"/>
       <c r="B22" s="34" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="37"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="34" t="s">
         <v>64</v>
       </c>
@@ -1256,7 +1471,7 @@
       <c r="B24" s="7"/>
     </row>
     <row r="25" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A25" s="37">
+      <c r="A25" s="40">
         <v>4</v>
       </c>
       <c r="B25" s="10" t="s">
@@ -1264,61 +1479,61 @@
       </c>
     </row>
     <row r="26" spans="1:2" ht="24" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="37"/>
+      <c r="A26" s="40"/>
       <c r="B26" s="23" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="24" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="37"/>
+      <c r="A27" s="40"/>
       <c r="B27" s="23" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="37"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="21" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="37"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="34" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="37"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="34" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="37"/>
+      <c r="A31" s="40"/>
       <c r="B31" s="34" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="37"/>
+      <c r="A32" s="40"/>
       <c r="B32" s="34" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="37"/>
+      <c r="A33" s="40"/>
       <c r="B33" s="34" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="37"/>
+      <c r="A34" s="40"/>
       <c r="B34" s="34" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="37"/>
+      <c r="A35" s="40"/>
       <c r="B35" s="34" t="s">
         <v>64</v>
       </c>
@@ -1358,7 +1573,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" ht="24" x14ac:dyDescent="0.3">
-      <c r="B43" s="51" t="s">
+      <c r="B43" s="38" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1373,7 +1588,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B46" s="49" t="s">
+      <c r="B46" s="36" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1388,7 +1603,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B49" s="50" t="s">
+      <c r="B49" s="37" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1710,10 +1925,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="48" t="s">
         <v>79</v>
       </c>
       <c r="C2" s="19" t="s">
@@ -1721,17 +1936,17 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="44"/>
-      <c r="B3" s="46"/>
+      <c r="A3" s="47"/>
+      <c r="B3" s="49"/>
       <c r="C3" s="19" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="46" t="s">
         <v>100</v>
       </c>
       <c r="C4" s="19" t="s">
@@ -1739,31 +1954,31 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="44"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="40" t="s">
+      <c r="A5" s="47"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="43" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="44"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="40"/>
+      <c r="C6" s="43"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="47"/>
+      <c r="A7" s="50"/>
       <c r="B7" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C7" s="40"/>
+      <c r="C7" s="43"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="51" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="51" t="s">
         <v>91</v>
       </c>
       <c r="C8" s="19" t="s">
@@ -1771,17 +1986,17 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="48"/>
-      <c r="B9" s="48"/>
+      <c r="A9" s="51"/>
+      <c r="B9" s="51"/>
       <c r="C9" s="19" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="44" t="s">
         <v>104</v>
       </c>
       <c r="C10" s="19" t="s">
@@ -1789,22 +2004,22 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="36"/>
-      <c r="B11" s="42"/>
+      <c r="A11" s="39"/>
+      <c r="B11" s="45"/>
       <c r="C11" s="19" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="36"/>
-      <c r="B12" s="42"/>
+      <c r="A12" s="39"/>
+      <c r="B12" s="45"/>
       <c r="C12" s="19" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="36"/>
-      <c r="B13" s="42"/>
+      <c r="A13" s="39"/>
+      <c r="B13" s="45"/>
       <c r="C13" s="19" t="s">
         <v>28</v>
       </c>
@@ -1961,6 +2176,441 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{151B78CE-323D-654A-8F0D-1D95D838F0AB}">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="47" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="53" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="54" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="55">
+        <v>1</v>
+      </c>
+      <c r="B2" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="56" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="57">
+        <v>100</v>
+      </c>
+      <c r="E2" s="58">
+        <v>98</v>
+      </c>
+      <c r="F2" s="59">
+        <v>102</v>
+      </c>
+      <c r="G2" s="60"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="61">
+        <v>2</v>
+      </c>
+      <c r="B3" s="56" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" s="57">
+        <v>100</v>
+      </c>
+      <c r="E3" s="59">
+        <v>102</v>
+      </c>
+      <c r="F3" s="58">
+        <v>98</v>
+      </c>
+      <c r="G3" s="60"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="61">
+        <v>3</v>
+      </c>
+      <c r="B4" s="56" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="56" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="57">
+        <v>100</v>
+      </c>
+      <c r="E4" s="57">
+        <v>100</v>
+      </c>
+      <c r="F4" s="58">
+        <v>98</v>
+      </c>
+      <c r="G4" s="60"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="61">
+        <v>4</v>
+      </c>
+      <c r="B5" s="56" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="57">
+        <v>100</v>
+      </c>
+      <c r="E5" s="58">
+        <v>98</v>
+      </c>
+      <c r="F5" s="57">
+        <v>100</v>
+      </c>
+      <c r="G5" s="60"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="61">
+        <v>5</v>
+      </c>
+      <c r="B6" s="56" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6" s="56" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" s="57">
+        <v>100</v>
+      </c>
+      <c r="E6" s="57">
+        <v>100</v>
+      </c>
+      <c r="F6" s="59">
+        <v>102</v>
+      </c>
+      <c r="G6" s="60"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="61">
+        <v>6</v>
+      </c>
+      <c r="B7" s="56" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" s="57">
+        <v>100</v>
+      </c>
+      <c r="E7" s="59">
+        <v>102</v>
+      </c>
+      <c r="F7" s="57">
+        <v>100</v>
+      </c>
+      <c r="G7" s="60"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="78"/>
+      <c r="B8" s="62" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" s="56" t="s">
+        <v>128</v>
+      </c>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="64" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="78"/>
+      <c r="B9" s="65" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" s="56" t="s">
+        <v>128</v>
+      </c>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="64" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="78"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="64" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="78"/>
+      <c r="B11" s="68" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="76" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="63"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="64" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="78"/>
+      <c r="B12" s="62" t="s">
+        <v>127</v>
+      </c>
+      <c r="C12" s="77"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="64" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="55">
+        <v>7</v>
+      </c>
+      <c r="B13" s="56" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" s="56" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" s="57">
+        <v>100</v>
+      </c>
+      <c r="E13" s="59">
+        <v>102</v>
+      </c>
+      <c r="F13" s="69">
+        <v>105</v>
+      </c>
+      <c r="G13" s="60"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="61">
+        <v>8</v>
+      </c>
+      <c r="B14" s="56" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="D14" s="57">
+        <v>100</v>
+      </c>
+      <c r="E14" s="69">
+        <v>105</v>
+      </c>
+      <c r="F14" s="59">
+        <v>102</v>
+      </c>
+      <c r="G14" s="60"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="78"/>
+      <c r="B15" s="70" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" s="56" t="s">
+        <v>128</v>
+      </c>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="64" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="78"/>
+      <c r="B16" s="71"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="64" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="78"/>
+      <c r="B17" s="68" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="76" t="s">
+        <v>114</v>
+      </c>
+      <c r="D17" s="63"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="64" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="78"/>
+      <c r="B18" s="65" t="s">
+        <v>129</v>
+      </c>
+      <c r="C18" s="77"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="63"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="64" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="55">
+        <v>9</v>
+      </c>
+      <c r="B19" s="56" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" s="56" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19" s="57">
+        <v>100</v>
+      </c>
+      <c r="E19" s="58">
+        <v>98</v>
+      </c>
+      <c r="F19" s="72">
+        <v>90</v>
+      </c>
+      <c r="G19" s="60"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="61">
+        <v>10</v>
+      </c>
+      <c r="B20" s="56" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20" s="57">
+        <v>100</v>
+      </c>
+      <c r="E20" s="72">
+        <v>90</v>
+      </c>
+      <c r="F20" s="58">
+        <v>98</v>
+      </c>
+      <c r="G20" s="60"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="78"/>
+      <c r="B21" s="70" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21" s="73" t="s">
+        <v>128</v>
+      </c>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="64" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="78"/>
+      <c r="B22" s="71"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="64" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="78"/>
+      <c r="B23" s="68" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="74" t="s">
+        <v>114</v>
+      </c>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="64" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="55">
+        <v>11</v>
+      </c>
+      <c r="B24" s="72" t="s">
+        <v>132</v>
+      </c>
+      <c r="C24" s="75" t="s">
+        <v>133</v>
+      </c>
+      <c r="D24" s="60"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="60"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C17:C18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16A524B1-76DA-D149-A83D-2FF66E4D844B}">
   <dimension ref="A1:B3"/>
   <sheetViews>

</xml_diff>

<commit_message>
test specs for leaderboard func complete through scenario 5
</commit_message>
<xml_diff>
--- a/excel-docs/euro - lifecycle info.xlsx
+++ b/excel-docs/euro - lifecycle info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joseph.collins/Documents/personal-projects/euro/2024_euro/excel-docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9196DE-BF60-0244-8F66-37138810B7F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3735654-95AC-FC43-B9BC-E383BDFF42DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20060" activeTab="3" xr2:uid="{D89656BD-B983-D041-A997-C1184058734E}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="life cycle actions" sheetId="6" r:id="rId1"/>
     <sheet name="part scenarios" sheetId="4" r:id="rId2"/>
     <sheet name="error testing" sheetId="3" r:id="rId3"/>
-    <sheet name="tiebreaker testing scneari" sheetId="8" r:id="rId4"/>
+    <sheet name="tiebreaker testing scenarios" sheetId="8" r:id="rId4"/>
     <sheet name="emails" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -2180,7 +2180,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updates to leaderboard complete
</commit_message>
<xml_diff>
--- a/excel-docs/euro - lifecycle info.xlsx
+++ b/excel-docs/euro - lifecycle info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joseph.collins/Documents/personal-projects/euro/2024_euro/excel-docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3735654-95AC-FC43-B9BC-E383BDFF42DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D56F65-7A0F-E64E-A551-EA6A10A9F14F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20060" activeTab="3" xr2:uid="{D89656BD-B983-D041-A997-C1184058734E}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20060" xr2:uid="{D89656BD-B983-D041-A997-C1184058734E}"/>
   </bookViews>
   <sheets>
     <sheet name="life cycle actions" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="135">
   <si>
     <t>need to submit a number for tiebreaker score</t>
   </si>
@@ -527,6 +527,13 @@
   </si>
   <si>
     <t>throw error</t>
+  </si>
+  <si>
+    <t>find the team with the longest name, and make sure all looks well with the following pages:
+groupDetails
+myPicks locked
+myPicks unlocked
+KO stages</t>
   </si>
 </sst>
 </file>
@@ -803,7 +810,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -873,45 +880,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -978,13 +946,56 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1008,7 +1019,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1296,7 +1307,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1307,10 +1318,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:F105"/>
+  <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" zoomScale="160" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1332,566 +1343,573 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="39">
+    <row r="2" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="73">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="80"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="74"/>
+      <c r="B3" s="32" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="39"/>
-      <c r="B3" s="32" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="74"/>
+      <c r="B4" s="32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="39"/>
-      <c r="B4" s="32" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="74"/>
+      <c r="B5" s="32" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="39"/>
-      <c r="B5" s="32" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="79"/>
+      <c r="B6" s="32" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="15"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="41">
+    <row r="7" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="15"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="66">
         <v>2</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B8" s="32" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="42"/>
-      <c r="B8" s="33" t="s">
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="67"/>
+      <c r="B9" s="33" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="40">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="65">
         <v>3</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B11" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="24" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="40"/>
-      <c r="B11" s="23" t="s">
+    <row r="12" spans="1:6" ht="24" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="65"/>
+      <c r="B12" s="23" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="24" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="40"/>
-      <c r="B12" s="23" t="s">
+    <row r="13" spans="1:6" ht="24" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="65"/>
+      <c r="B13" s="23" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="40"/>
-      <c r="B13" s="34" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="65"/>
+      <c r="B14" s="34" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="40"/>
-      <c r="B14" s="34" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="65"/>
+      <c r="B15" s="34" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="40"/>
-      <c r="B15" s="34" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="65"/>
+      <c r="B16" s="34" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="40"/>
-      <c r="B16" s="34" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="65"/>
+      <c r="B17" s="34" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="40"/>
-      <c r="B17" s="34" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="65"/>
+      <c r="B18" s="34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="40"/>
-      <c r="B18" s="34" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="65"/>
+      <c r="B19" s="34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="40"/>
-      <c r="B19" s="34" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="65"/>
+      <c r="B20" s="34" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="40"/>
-      <c r="B20" s="34" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="65"/>
+      <c r="B21" s="34" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="40"/>
-      <c r="B21" s="34" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="65"/>
+      <c r="B22" s="34" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="40"/>
-      <c r="B22" s="34" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="65"/>
+      <c r="B23" s="34" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="40"/>
-      <c r="B23" s="34" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="65"/>
+      <c r="B24" s="34" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="6"/>
-      <c r="B24" s="7"/>
-    </row>
-    <row r="25" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A25" s="40">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="6"/>
+      <c r="B25" s="7"/>
+    </row>
+    <row r="26" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A26" s="65">
         <v>4</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B26" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="24" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="40"/>
-      <c r="B26" s="23" t="s">
+    <row r="27" spans="1:2" ht="24" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="65"/>
+      <c r="B27" s="23" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="24" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="40"/>
-      <c r="B27" s="23" t="s">
+    <row r="28" spans="1:2" ht="24" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="65"/>
+      <c r="B28" s="23" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="40"/>
-      <c r="B28" s="21" t="s">
+    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="65"/>
+      <c r="B29" s="21" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="40"/>
-      <c r="B29" s="34" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="65"/>
+      <c r="B30" s="34" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="40"/>
-      <c r="B30" s="34" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="65"/>
+      <c r="B31" s="34" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="40"/>
-      <c r="B31" s="34" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="65"/>
+      <c r="B32" s="34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="40"/>
-      <c r="B32" s="34" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="65"/>
+      <c r="B33" s="34" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="40"/>
-      <c r="B33" s="34" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="65"/>
+      <c r="B34" s="34" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="40"/>
-      <c r="B34" s="34" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="65"/>
+      <c r="B35" s="34" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="40"/>
-      <c r="B35" s="34" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="65"/>
+      <c r="B36" s="34" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="6"/>
-      <c r="B36" s="7"/>
-    </row>
-    <row r="37" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="B37" s="10" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="6"/>
+      <c r="B37" s="7"/>
+    </row>
+    <row r="38" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="B38" s="10" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B38" s="32" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B39" s="32" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B40" s="32" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B41" s="32" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="25" t="s">
+    <row r="42" spans="1:2" ht="21" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="25" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="24" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="23" t="s">
+    <row r="43" spans="1:2" ht="24" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="23" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="24" x14ac:dyDescent="0.3">
-      <c r="B43" s="38" t="s">
+    <row r="44" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="B44" s="38" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B44" s="32" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B45" s="32" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B45" s="34" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B46" s="34" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B46" s="36" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B47" s="36" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B47" s="34" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B48" s="34" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B49" s="34" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B49" s="37" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B50" s="37" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B50" s="34" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B51" s="34" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B52" s="34" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B53" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C52" s="9"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="6"/>
-      <c r="B53" s="7"/>
-    </row>
-    <row r="54" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="B54" s="10" t="s">
+      <c r="C53" s="9"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="6"/>
+      <c r="B54" s="7"/>
+    </row>
+    <row r="55" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="B55" s="10" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B55" s="21" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B56" s="21" t="s">
-        <v>105</v>
+        <v>68</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B57" s="21" t="s">
-        <v>37</v>
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B58" s="21" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B59" s="21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B60" s="21" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B60" s="24" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B61" s="24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B61" s="26" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B62" s="26" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B62" s="24" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B63" s="24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B64" s="24" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B64" s="27" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B65" s="27" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B65" s="22" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B66" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B67" s="22" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B67" s="24" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B68" s="24" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" s="6"/>
-      <c r="B68" s="7"/>
-    </row>
-    <row r="69" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="B69" s="10" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="6"/>
+      <c r="B69" s="7"/>
+    </row>
+    <row r="70" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="B70" s="10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B70" s="21" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B71" s="21" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="24" x14ac:dyDescent="0.3">
-      <c r="B71" s="23" t="s">
+    <row r="72" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="B72" s="23" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="31" t="s">
+    <row r="73" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="31" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B73" s="21" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B74" s="21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B75" s="21" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B75" s="24" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B76" s="24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B76" s="26" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B77" s="26" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B77" s="24" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B78" s="24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B79" s="24" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B79" s="27" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B80" s="27" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B80" s="22" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B81" s="22" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B82" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B83" s="22" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B84" s="22" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B85" s="22" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B85" s="24" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B86" s="24" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="6"/>
-      <c r="B86" s="7"/>
-    </row>
-    <row r="87" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="B87" s="10" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="6"/>
+      <c r="B87" s="7"/>
+    </row>
+    <row r="88" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="B88" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B88" s="21" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B89" s="21" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="24" x14ac:dyDescent="0.3">
-      <c r="B89" s="23" t="s">
+    <row r="90" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="B90" s="23" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B90" s="24" t="s">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B91" s="24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B91" s="26" t="s">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B92" s="26" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B92" s="24" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B93" s="24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B94" s="24" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B94" s="22" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B95" s="22" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B96" s="22" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B97" s="22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B98" s="22" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B98" s="24" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B99" s="24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B100" s="24" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="6"/>
-      <c r="B100" s="7"/>
-    </row>
-    <row r="101" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="B101" s="10" t="s">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="6"/>
+      <c r="B101" s="7"/>
+    </row>
+    <row r="102" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="B102" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="102" spans="1:2" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.3">
-      <c r="A102" s="29"/>
-      <c r="B102" s="23" t="s">
+    <row r="103" spans="1:2" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A103" s="29"/>
+      <c r="B103" s="23" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="103" spans="1:2" s="13" customFormat="1" ht="24" x14ac:dyDescent="0.3">
-      <c r="A103" s="30"/>
-      <c r="B103" s="23" t="s">
+    <row r="104" spans="1:2" s="13" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A104" s="30"/>
+      <c r="B104" s="23" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B104" s="21" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B105" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B106" s="21" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A10:A23"/>
-    <mergeCell ref="A25:A35"/>
-    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A11:A24"/>
+    <mergeCell ref="A26:A36"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A2:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1925,10 +1943,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="73" t="s">
         <v>79</v>
       </c>
       <c r="C2" s="19" t="s">
@@ -1936,17 +1954,17 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="47"/>
-      <c r="B3" s="49"/>
+      <c r="A3" s="72"/>
+      <c r="B3" s="74"/>
       <c r="C3" s="19" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="71" t="s">
         <v>100</v>
       </c>
       <c r="C4" s="19" t="s">
@@ -1954,31 +1972,31 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="47"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="43" t="s">
+      <c r="A5" s="72"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="68" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="47"/>
+      <c r="A6" s="72"/>
       <c r="B6" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="43"/>
+      <c r="C6" s="68"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="50"/>
+      <c r="A7" s="75"/>
       <c r="B7" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C7" s="43"/>
+      <c r="C7" s="68"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="76" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="76" t="s">
         <v>91</v>
       </c>
       <c r="C8" s="19" t="s">
@@ -1986,17 +2004,17 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="51"/>
-      <c r="B9" s="51"/>
+      <c r="A9" s="76"/>
+      <c r="B9" s="76"/>
       <c r="C9" s="19" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="64" t="s">
         <v>98</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="69" t="s">
         <v>104</v>
       </c>
       <c r="C10" s="19" t="s">
@@ -2004,22 +2022,22 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="39"/>
-      <c r="B11" s="45"/>
+      <c r="A11" s="64"/>
+      <c r="B11" s="70"/>
       <c r="C11" s="19" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="39"/>
-      <c r="B12" s="45"/>
+      <c r="A12" s="64"/>
+      <c r="B12" s="70"/>
       <c r="C12" s="19" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="39"/>
-      <c r="B13" s="45"/>
+      <c r="A13" s="64"/>
+      <c r="B13" s="70"/>
       <c r="C13" s="19" t="s">
         <v>28</v>
       </c>
@@ -2179,7 +2197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{151B78CE-323D-654A-8F0D-1D95D838F0AB}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
@@ -2190,416 +2208,416 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="F1" s="54" t="s">
+      <c r="F1" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="G1" s="54" t="s">
+      <c r="G1" s="41" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="55">
+      <c r="A2" s="42">
         <v>1</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="D2" s="57">
+      <c r="D2" s="44">
         <v>100</v>
       </c>
-      <c r="E2" s="58">
+      <c r="E2" s="45">
         <v>98</v>
       </c>
-      <c r="F2" s="59">
+      <c r="F2" s="46">
         <v>102</v>
       </c>
-      <c r="G2" s="60"/>
+      <c r="G2" s="47"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="61">
+      <c r="A3" s="48">
         <v>2</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="D3" s="57">
+      <c r="D3" s="44">
         <v>100</v>
       </c>
-      <c r="E3" s="59">
+      <c r="E3" s="46">
         <v>102</v>
       </c>
-      <c r="F3" s="58">
+      <c r="F3" s="45">
         <v>98</v>
       </c>
-      <c r="G3" s="60"/>
+      <c r="G3" s="47"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="61">
+      <c r="A4" s="48">
         <v>3</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="D4" s="57">
+      <c r="D4" s="44">
         <v>100</v>
       </c>
-      <c r="E4" s="57">
+      <c r="E4" s="44">
         <v>100</v>
       </c>
-      <c r="F4" s="58">
+      <c r="F4" s="45">
         <v>98</v>
       </c>
-      <c r="G4" s="60"/>
+      <c r="G4" s="47"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="61">
+      <c r="A5" s="48">
         <v>4</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="D5" s="57">
+      <c r="D5" s="44">
         <v>100</v>
       </c>
-      <c r="E5" s="58">
+      <c r="E5" s="45">
         <v>98</v>
       </c>
-      <c r="F5" s="57">
+      <c r="F5" s="44">
         <v>100</v>
       </c>
-      <c r="G5" s="60"/>
+      <c r="G5" s="47"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="61">
+      <c r="A6" s="48">
         <v>5</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="C6" s="56" t="s">
+      <c r="C6" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="D6" s="57">
+      <c r="D6" s="44">
         <v>100</v>
       </c>
-      <c r="E6" s="57">
+      <c r="E6" s="44">
         <v>100</v>
       </c>
-      <c r="F6" s="59">
+      <c r="F6" s="46">
         <v>102</v>
       </c>
-      <c r="G6" s="60"/>
+      <c r="G6" s="47"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="61">
+      <c r="A7" s="48">
         <v>6</v>
       </c>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="C7" s="56" t="s">
+      <c r="C7" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="D7" s="57">
+      <c r="D7" s="44">
         <v>100</v>
       </c>
-      <c r="E7" s="59">
+      <c r="E7" s="46">
         <v>102</v>
       </c>
-      <c r="F7" s="57">
+      <c r="F7" s="44">
         <v>100</v>
       </c>
-      <c r="G7" s="60"/>
+      <c r="G7" s="47"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="78"/>
-      <c r="B8" s="62" t="s">
+      <c r="A8" s="63"/>
+      <c r="B8" s="49" t="s">
         <v>127</v>
       </c>
-      <c r="C8" s="56" t="s">
+      <c r="C8" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="64" t="s">
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="51" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="78"/>
-      <c r="B9" s="65" t="s">
+      <c r="A9" s="63"/>
+      <c r="B9" s="52" t="s">
         <v>129</v>
       </c>
-      <c r="C9" s="56" t="s">
+      <c r="C9" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="64" t="s">
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="51" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="78"/>
-      <c r="B10" s="66"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="64" t="s">
+      <c r="A10" s="63"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="51" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="78"/>
-      <c r="B11" s="68" t="s">
+      <c r="A11" s="63"/>
+      <c r="B11" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="76" t="s">
+      <c r="C11" s="77" t="s">
         <v>114</v>
       </c>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="64" t="s">
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="51" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="78"/>
-      <c r="B12" s="62" t="s">
+      <c r="A12" s="63"/>
+      <c r="B12" s="49" t="s">
         <v>127</v>
       </c>
-      <c r="C12" s="77"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="64" t="s">
+      <c r="C12" s="78"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="51" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="55">
+      <c r="A13" s="42">
         <v>7</v>
       </c>
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="C13" s="56" t="s">
+      <c r="C13" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="D13" s="57">
+      <c r="D13" s="44">
         <v>100</v>
       </c>
-      <c r="E13" s="59">
+      <c r="E13" s="46">
         <v>102</v>
       </c>
-      <c r="F13" s="69">
+      <c r="F13" s="56">
         <v>105</v>
       </c>
-      <c r="G13" s="60"/>
+      <c r="G13" s="47"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="61">
+      <c r="A14" s="48">
         <v>8</v>
       </c>
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="43" t="s">
         <v>131</v>
       </c>
-      <c r="C14" s="56" t="s">
+      <c r="C14" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="D14" s="57">
+      <c r="D14" s="44">
         <v>100</v>
       </c>
-      <c r="E14" s="69">
+      <c r="E14" s="56">
         <v>105</v>
       </c>
-      <c r="F14" s="59">
+      <c r="F14" s="46">
         <v>102</v>
       </c>
-      <c r="G14" s="60"/>
+      <c r="G14" s="47"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="78"/>
-      <c r="B15" s="70" t="s">
+      <c r="A15" s="63"/>
+      <c r="B15" s="57" t="s">
         <v>132</v>
       </c>
-      <c r="C15" s="56" t="s">
+      <c r="C15" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="64" t="s">
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="51" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="78"/>
-      <c r="B16" s="71"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="64" t="s">
+      <c r="A16" s="63"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="51" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="78"/>
-      <c r="B17" s="68" t="s">
+      <c r="A17" s="63"/>
+      <c r="B17" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="76" t="s">
+      <c r="C17" s="77" t="s">
         <v>114</v>
       </c>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="64" t="s">
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="51" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="78"/>
-      <c r="B18" s="65" t="s">
+      <c r="A18" s="63"/>
+      <c r="B18" s="52" t="s">
         <v>129</v>
       </c>
-      <c r="C18" s="77"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="63"/>
-      <c r="G18" s="64" t="s">
+      <c r="C18" s="78"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="51" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="55">
+      <c r="A19" s="42">
         <v>9</v>
       </c>
-      <c r="B19" s="56" t="s">
+      <c r="B19" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="C19" s="56" t="s">
+      <c r="C19" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="D19" s="57">
+      <c r="D19" s="44">
         <v>100</v>
       </c>
-      <c r="E19" s="58">
+      <c r="E19" s="45">
         <v>98</v>
       </c>
-      <c r="F19" s="72">
+      <c r="F19" s="59">
         <v>90</v>
       </c>
-      <c r="G19" s="60"/>
+      <c r="G19" s="47"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="61">
+      <c r="A20" s="48">
         <v>10</v>
       </c>
-      <c r="B20" s="56" t="s">
+      <c r="B20" s="43" t="s">
         <v>131</v>
       </c>
-      <c r="C20" s="56" t="s">
+      <c r="C20" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="D20" s="57">
+      <c r="D20" s="44">
         <v>100</v>
       </c>
-      <c r="E20" s="72">
+      <c r="E20" s="59">
         <v>90</v>
       </c>
-      <c r="F20" s="58">
+      <c r="F20" s="45">
         <v>98</v>
       </c>
-      <c r="G20" s="60"/>
+      <c r="G20" s="47"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="78"/>
-      <c r="B21" s="70" t="s">
+      <c r="A21" s="63"/>
+      <c r="B21" s="57" t="s">
         <v>132</v>
       </c>
-      <c r="C21" s="73" t="s">
+      <c r="C21" s="60" t="s">
         <v>128</v>
       </c>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="64" t="s">
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="78"/>
-      <c r="B22" s="71"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
-      <c r="F22" s="60"/>
-      <c r="G22" s="64" t="s">
+      <c r="A22" s="63"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="51" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="78"/>
-      <c r="B23" s="68" t="s">
+      <c r="A23" s="63"/>
+      <c r="B23" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="74" t="s">
+      <c r="C23" s="61" t="s">
         <v>114</v>
       </c>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="64" t="s">
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="51" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="55">
+      <c r="A24" s="42">
         <v>11</v>
       </c>
-      <c r="B24" s="72" t="s">
+      <c r="B24" s="59" t="s">
         <v>132</v>
       </c>
-      <c r="C24" s="75" t="s">
+      <c r="C24" s="62" t="s">
         <v>133</v>
       </c>
-      <c r="D24" s="60"/>
-      <c r="E24" s="60"/>
-      <c r="F24" s="60"/>
-      <c r="G24" s="60"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
determing round of 16 matchups complete
</commit_message>
<xml_diff>
--- a/excel-docs/euro - lifecycle info.xlsx
+++ b/excel-docs/euro - lifecycle info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joseph.collins/Documents/personal-projects/euro/2024_euro/excel-docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB45C74-F9F8-E949-ACCA-42E26FFE96FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424B29E7-C1DE-CA4D-A386-1CCB135BF4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34560" yWindow="500" windowWidth="38400" windowHeight="21100" firstSheet="4" activeTab="10" xr2:uid="{D89656BD-B983-D041-A997-C1184058734E}"/>
+    <workbookView xWindow="23300" yWindow="1760" windowWidth="10000" windowHeight="20120" firstSheet="8" activeTab="11" xr2:uid="{D89656BD-B983-D041-A997-C1184058734E}"/>
   </bookViews>
   <sheets>
     <sheet name="life cycle actions" sheetId="6" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="kevin" sheetId="13" r:id="rId9"/>
     <sheet name="sarah" sheetId="14" r:id="rId10"/>
     <sheet name="pat" sheetId="15" r:id="rId11"/>
+    <sheet name="ko" sheetId="16" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="247">
   <si>
     <t>need to submit a number for tiebreaker score</t>
   </si>
@@ -722,6 +723,159 @@
   </si>
   <si>
     <t>kevin - group D</t>
+  </si>
+  <si>
+    <t>belgium</t>
+  </si>
+  <si>
+    <t>portugal</t>
+  </si>
+  <si>
+    <t>italy</t>
+  </si>
+  <si>
+    <t>austria</t>
+  </si>
+  <si>
+    <t>switz</t>
+  </si>
+  <si>
+    <t>croatia</t>
+  </si>
+  <si>
+    <t>spain</t>
+  </si>
+  <si>
+    <t>sweden</t>
+  </si>
+  <si>
+    <t>ukraine</t>
+  </si>
+  <si>
+    <t>england</t>
+  </si>
+  <si>
+    <t>germany</t>
+  </si>
+  <si>
+    <t>dutch</t>
+  </si>
+  <si>
+    <t>czech</t>
+  </si>
+  <si>
+    <t>wales</t>
+  </si>
+  <si>
+    <t>denmark</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>france</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>absolute match-ups</t>
+  </si>
+  <si>
+    <t>euro 2020</t>
+  </si>
+  <si>
+    <t>Dutch</t>
+  </si>
+  <si>
+    <t>senegal</t>
+  </si>
+  <si>
+    <t>argentina</t>
+  </si>
+  <si>
+    <t>mexico</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>Q6</t>
+  </si>
+  <si>
+    <t>Q7</t>
+  </si>
+  <si>
+    <t>Q8</t>
+  </si>
+  <si>
+    <t>ACDE mock testing</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>poland</t>
+  </si>
+  <si>
+    <t>austrailia</t>
+  </si>
+  <si>
+    <t>japan</t>
   </si>
 </sst>
 </file>
@@ -1038,7 +1192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1215,6 +1369,8 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1264,6 +1420,22 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1504,9 +1676,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF180F1A"/>
       <color rgb="FFFF2FB7"/>
       <color rgb="FFBE1FFF"/>
-      <color rgb="FF180F1A"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1846,7 +2018,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="85">
+      <c r="A2" s="87">
         <v>1</v>
       </c>
       <c r="B2" s="33" t="s">
@@ -1854,25 +2026,25 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="86"/>
+      <c r="A3" s="88"/>
       <c r="B3" s="32" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="86"/>
+      <c r="A4" s="88"/>
       <c r="B4" s="32" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="86"/>
+      <c r="A5" s="88"/>
       <c r="B5" s="32" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="87"/>
+      <c r="A6" s="89"/>
       <c r="B6" s="32" t="s">
         <v>16</v>
       </c>
@@ -1882,7 +2054,7 @@
       <c r="B7" s="15"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="83">
+      <c r="A8" s="85">
         <v>2</v>
       </c>
       <c r="B8" s="32" t="s">
@@ -1890,7 +2062,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="84"/>
+      <c r="A9" s="86"/>
       <c r="B9" s="33" t="s">
         <v>94</v>
       </c>
@@ -1900,7 +2072,7 @@
       <c r="B10" s="7"/>
     </row>
     <row r="11" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="82">
+      <c r="A11" s="84">
         <v>3</v>
       </c>
       <c r="B11" s="10" t="s">
@@ -1908,79 +2080,79 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="24" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="82"/>
+      <c r="A12" s="84"/>
       <c r="B12" s="23" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="24" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="82"/>
+      <c r="A13" s="84"/>
       <c r="B13" s="23" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="82"/>
+      <c r="A14" s="84"/>
       <c r="B14" s="34" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="82"/>
+      <c r="A15" s="84"/>
       <c r="B15" s="34" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="82"/>
+      <c r="A16" s="84"/>
       <c r="B16" s="34" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="82"/>
+      <c r="A17" s="84"/>
       <c r="B17" s="34" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="82"/>
+      <c r="A18" s="84"/>
       <c r="B18" s="34" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="82"/>
+      <c r="A19" s="84"/>
       <c r="B19" s="34" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="82"/>
+      <c r="A20" s="84"/>
       <c r="B20" s="34" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="82"/>
+      <c r="A21" s="84"/>
       <c r="B21" s="34" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="82"/>
+      <c r="A22" s="84"/>
       <c r="B22" s="34" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="82"/>
+      <c r="A23" s="84"/>
       <c r="B23" s="34" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="82"/>
+      <c r="A24" s="84"/>
       <c r="B24" s="34" t="s">
         <v>64</v>
       </c>
@@ -1990,7 +2162,7 @@
       <c r="B25" s="7"/>
     </row>
     <row r="26" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A26" s="82">
+      <c r="A26" s="84">
         <v>4</v>
       </c>
       <c r="B26" s="10" t="s">
@@ -1998,61 +2170,61 @@
       </c>
     </row>
     <row r="27" spans="1:2" ht="24" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="82"/>
+      <c r="A27" s="84"/>
       <c r="B27" s="23" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="24" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="82"/>
+      <c r="A28" s="84"/>
       <c r="B28" s="23" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="82"/>
+      <c r="A29" s="84"/>
       <c r="B29" s="21" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="82"/>
+      <c r="A30" s="84"/>
       <c r="B30" s="34" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="82"/>
+      <c r="A31" s="84"/>
       <c r="B31" s="34" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="82"/>
+      <c r="A32" s="84"/>
       <c r="B32" s="34" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="82"/>
+      <c r="A33" s="84"/>
       <c r="B33" s="34" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="82"/>
+      <c r="A34" s="84"/>
       <c r="B34" s="34" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="82"/>
+      <c r="A35" s="84"/>
       <c r="B35" s="34" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="82"/>
+      <c r="A36" s="84"/>
       <c r="B36" s="34" t="s">
         <v>64</v>
       </c>
@@ -2453,14 +2625,14 @@
       <c r="A2" s="70">
         <v>5</v>
       </c>
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="100" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
@@ -2475,14 +2647,14 @@
       <c r="A3" s="78">
         <v>4</v>
       </c>
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>142</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
@@ -2497,14 +2669,14 @@
       <c r="A4" s="73">
         <v>3</v>
       </c>
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="100" t="s">
         <v>144</v>
       </c>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
@@ -2519,14 +2691,14 @@
       <c r="A5" s="79">
         <v>2</v>
       </c>
-      <c r="B5" s="98" t="s">
+      <c r="B5" s="100" t="s">
         <v>145</v>
       </c>
-      <c r="C5" s="98"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="98"/>
-      <c r="F5" s="98"/>
-      <c r="G5" s="98"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
@@ -2541,14 +2713,14 @@
       <c r="A6" s="71">
         <v>1</v>
       </c>
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="100" t="s">
         <v>146</v>
       </c>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="98"/>
-      <c r="G6" s="98"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="100"/>
+      <c r="F6" s="100"/>
+      <c r="G6" s="100"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
@@ -3550,7 +3722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08564AC3-4506-8F41-9905-B73B2E25376A}">
   <dimension ref="A1:AA34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -3583,14 +3755,14 @@
       <c r="A2" s="70">
         <v>5</v>
       </c>
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="100" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
@@ -3605,14 +3777,14 @@
       <c r="A3" s="78">
         <v>4</v>
       </c>
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>142</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
@@ -3627,14 +3799,14 @@
       <c r="A4" s="73">
         <v>3</v>
       </c>
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="100" t="s">
         <v>144</v>
       </c>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
@@ -3649,14 +3821,14 @@
       <c r="A5" s="79">
         <v>2</v>
       </c>
-      <c r="B5" s="98" t="s">
+      <c r="B5" s="100" t="s">
         <v>145</v>
       </c>
-      <c r="C5" s="98"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="98"/>
-      <c r="F5" s="98"/>
-      <c r="G5" s="98"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
@@ -3671,14 +3843,14 @@
       <c r="A6" s="71">
         <v>1</v>
       </c>
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="100" t="s">
         <v>146</v>
       </c>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="98"/>
-      <c r="G6" s="98"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="100"/>
+      <c r="F6" s="100"/>
+      <c r="G6" s="100"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
@@ -4676,6 +4848,419 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB61D7A-DE06-5C4A-93AA-F7A81E59FD2A}">
+  <dimension ref="A1:J27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="2.5" customWidth="1"/>
+    <col min="10" max="10" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I1" s="82"/>
+      <c r="J1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="105" t="s">
+        <v>229</v>
+      </c>
+      <c r="B2" s="105"/>
+      <c r="C2" s="105"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="B3" s="103" t="s">
+        <v>211</v>
+      </c>
+      <c r="C3" s="104" t="s">
+        <v>196</v>
+      </c>
+      <c r="D3" s="83"/>
+      <c r="E3" s="104" t="s">
+        <v>203</v>
+      </c>
+      <c r="F3" s="103" t="s">
+        <v>222</v>
+      </c>
+      <c r="G3" s="106" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="102"/>
+      <c r="B4" s="76" t="s">
+        <v>227</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="D4" s="83"/>
+      <c r="E4" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="F4" s="76" t="s">
+        <v>218</v>
+      </c>
+      <c r="G4" s="102"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="66"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="66"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="101" t="s">
+        <v>235</v>
+      </c>
+      <c r="B6" s="70" t="s">
+        <v>212</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="D6" s="83"/>
+      <c r="E6" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="F6" s="70" t="s">
+        <v>219</v>
+      </c>
+      <c r="G6" s="101" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="102"/>
+      <c r="B7" s="70" t="s">
+        <v>217</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="D7" s="83"/>
+      <c r="E7" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="F7" s="70" t="s">
+        <v>226</v>
+      </c>
+      <c r="G7" s="102"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="66"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="83"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="66"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="101" t="s">
+        <v>236</v>
+      </c>
+      <c r="B9" s="66" t="s">
+        <v>225</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D9" s="83"/>
+      <c r="E9" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="F9" s="66" t="s">
+        <v>216</v>
+      </c>
+      <c r="G9" s="101" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="102"/>
+      <c r="B10" s="76" t="s">
+        <v>214</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="D10" s="83"/>
+      <c r="E10" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="F10" s="76" t="s">
+        <v>221</v>
+      </c>
+      <c r="G10" s="102"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="66"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="83"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="66"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="101" t="s">
+        <v>237</v>
+      </c>
+      <c r="B12" s="70" t="s">
+        <v>220</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="D12" s="83"/>
+      <c r="E12" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="F12" s="70" t="s">
+        <v>213</v>
+      </c>
+      <c r="G12" s="101" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="102"/>
+      <c r="B13" s="70" t="s">
+        <v>223</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="D13" s="83"/>
+      <c r="E13" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="F13" s="70" t="s">
+        <v>215</v>
+      </c>
+      <c r="G13" s="102"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="105" t="s">
+        <v>242</v>
+      </c>
+      <c r="B16" s="105"/>
+      <c r="C16" s="105"/>
+      <c r="D16" s="105"/>
+      <c r="E16" s="105"/>
+      <c r="F16" s="105"/>
+      <c r="G16" s="105"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="101" t="s">
+        <v>234</v>
+      </c>
+      <c r="B17" s="103" t="s">
+        <v>211</v>
+      </c>
+      <c r="C17" s="104" t="s">
+        <v>161</v>
+      </c>
+      <c r="D17" s="83"/>
+      <c r="E17" s="104" t="s">
+        <v>206</v>
+      </c>
+      <c r="F17" s="103" t="s">
+        <v>222</v>
+      </c>
+      <c r="G17" s="101" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="102"/>
+      <c r="B18" s="76" t="s">
+        <v>243</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="D18" s="83"/>
+      <c r="E18" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="F18" s="76" t="s">
+        <v>218</v>
+      </c>
+      <c r="G18" s="102"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="66"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="83"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="66"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="101" t="s">
+        <v>235</v>
+      </c>
+      <c r="B20" s="70" t="s">
+        <v>212</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="D20" s="83"/>
+      <c r="E20" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="F20" s="70" t="s">
+        <v>219</v>
+      </c>
+      <c r="G20" s="101" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="102"/>
+      <c r="B21" s="70" t="s">
+        <v>217</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="D21" s="83"/>
+      <c r="E21" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="F21" s="70" t="s">
+        <v>226</v>
+      </c>
+      <c r="G21" s="102"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="66"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="83"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="66"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="101" t="s">
+        <v>236</v>
+      </c>
+      <c r="B23" s="66" t="s">
+        <v>225</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="D23" s="83"/>
+      <c r="E23" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="F23" s="66" t="s">
+        <v>216</v>
+      </c>
+      <c r="G23" s="101" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="102"/>
+      <c r="B24" s="76" t="s">
+        <v>214</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="D24" s="83"/>
+      <c r="E24" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="F24" s="76" t="s">
+        <v>221</v>
+      </c>
+      <c r="G24" s="102"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="66"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="83"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="66"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="101" t="s">
+        <v>237</v>
+      </c>
+      <c r="B26" s="70" t="s">
+        <v>220</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="D26" s="83"/>
+      <c r="E26" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="F26" s="70" t="s">
+        <v>213</v>
+      </c>
+      <c r="G26" s="101" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="102"/>
+      <c r="B27" s="70" t="s">
+        <v>223</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="D27" s="83"/>
+      <c r="E27" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="F27" s="70" t="s">
+        <v>215</v>
+      </c>
+      <c r="G27" s="102"/>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B757BA3-9E92-1F4D-A48F-D74F4F5BF1E1}">
   <dimension ref="A1:C13"/>
@@ -4704,10 +5289,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="87" t="s">
         <v>79</v>
       </c>
       <c r="C2" s="19" t="s">
@@ -4715,17 +5300,17 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="93"/>
-      <c r="B3" s="86"/>
+      <c r="A3" s="95"/>
+      <c r="B3" s="88"/>
       <c r="C3" s="19" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="92" t="s">
+      <c r="A4" s="94" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="92" t="s">
+      <c r="B4" s="94" t="s">
         <v>100</v>
       </c>
       <c r="C4" s="19" t="s">
@@ -4733,31 +5318,31 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="93"/>
-      <c r="B5" s="94"/>
-      <c r="C5" s="88" t="s">
+      <c r="A5" s="95"/>
+      <c r="B5" s="96"/>
+      <c r="C5" s="90" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="93"/>
+      <c r="A6" s="95"/>
       <c r="B6" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="88"/>
+      <c r="C6" s="90"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="94"/>
+      <c r="A7" s="96"/>
       <c r="B7" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C7" s="88"/>
+      <c r="C7" s="90"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="95" t="s">
+      <c r="A8" s="97" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="95" t="s">
+      <c r="B8" s="97" t="s">
         <v>91</v>
       </c>
       <c r="C8" s="19" t="s">
@@ -4765,17 +5350,17 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="95"/>
-      <c r="B9" s="95"/>
+      <c r="A9" s="97"/>
+      <c r="B9" s="97"/>
       <c r="C9" s="19" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="89" t="s">
+      <c r="A10" s="91" t="s">
         <v>98</v>
       </c>
-      <c r="B10" s="90" t="s">
+      <c r="B10" s="92" t="s">
         <v>104</v>
       </c>
       <c r="C10" s="19" t="s">
@@ -4783,22 +5368,22 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="89"/>
-      <c r="B11" s="91"/>
+      <c r="A11" s="91"/>
+      <c r="B11" s="93"/>
       <c r="C11" s="19" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="89"/>
-      <c r="B12" s="91"/>
+      <c r="A12" s="91"/>
+      <c r="B12" s="93"/>
       <c r="C12" s="19" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="89"/>
-      <c r="B13" s="91"/>
+      <c r="A13" s="91"/>
+      <c r="B13" s="93"/>
       <c r="C13" s="19" t="s">
         <v>28</v>
       </c>
@@ -5163,7 +5748,7 @@
       <c r="B11" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="96" t="s">
+      <c r="C11" s="98" t="s">
         <v>114</v>
       </c>
       <c r="D11" s="50"/>
@@ -5178,7 +5763,7 @@
       <c r="B12" s="49" t="s">
         <v>127</v>
       </c>
-      <c r="C12" s="97"/>
+      <c r="C12" s="99"/>
       <c r="D12" s="50"/>
       <c r="E12" s="50"/>
       <c r="F12" s="50"/>
@@ -5259,7 +5844,7 @@
       <c r="B17" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="96" t="s">
+      <c r="C17" s="98" t="s">
         <v>114</v>
       </c>
       <c r="D17" s="50"/>
@@ -5274,7 +5859,7 @@
       <c r="B18" s="52" t="s">
         <v>129</v>
       </c>
-      <c r="C18" s="97"/>
+      <c r="C18" s="99"/>
       <c r="D18" s="50"/>
       <c r="E18" s="50"/>
       <c r="F18" s="50"/>
@@ -5713,14 +6298,14 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="68"/>
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="100" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
@@ -5731,14 +6316,14 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="77"/>
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>142</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
@@ -5749,14 +6334,14 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="72"/>
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="100" t="s">
         <v>144</v>
       </c>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
@@ -5767,14 +6352,14 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="69"/>
-      <c r="B5" s="98" t="s">
+      <c r="B5" s="100" t="s">
         <v>145</v>
       </c>
-      <c r="C5" s="98"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="98"/>
-      <c r="F5" s="98"/>
-      <c r="G5" s="98"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
@@ -5785,14 +6370,14 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="22"/>
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="100" t="s">
         <v>146</v>
       </c>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="98"/>
-      <c r="G6" s="98"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="100"/>
+      <c r="F6" s="100"/>
+      <c r="G6" s="100"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
@@ -6773,14 +7358,14 @@
       <c r="A2" s="70">
         <v>5</v>
       </c>
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="100" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
@@ -6795,14 +7380,14 @@
       <c r="A3" s="78">
         <v>4</v>
       </c>
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>142</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
@@ -6817,14 +7402,14 @@
       <c r="A4" s="73">
         <v>3</v>
       </c>
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="100" t="s">
         <v>144</v>
       </c>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
@@ -6839,14 +7424,14 @@
       <c r="A5" s="79">
         <v>2</v>
       </c>
-      <c r="B5" s="98" t="s">
+      <c r="B5" s="100" t="s">
         <v>145</v>
       </c>
-      <c r="C5" s="98"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="98"/>
-      <c r="F5" s="98"/>
-      <c r="G5" s="98"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
@@ -6861,14 +7446,14 @@
       <c r="A6" s="71">
         <v>1</v>
       </c>
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="100" t="s">
         <v>146</v>
       </c>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="98"/>
-      <c r="G6" s="98"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="100"/>
+      <c r="F6" s="100"/>
+      <c r="G6" s="100"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
@@ -7968,14 +8553,14 @@
       <c r="A2" s="70">
         <v>5</v>
       </c>
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="100" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
@@ -7990,14 +8575,14 @@
       <c r="A3" s="78">
         <v>4</v>
       </c>
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>142</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
@@ -8012,14 +8597,14 @@
       <c r="A4" s="73">
         <v>3</v>
       </c>
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="100" t="s">
         <v>144</v>
       </c>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
@@ -8034,14 +8619,14 @@
       <c r="A5" s="79">
         <v>2</v>
       </c>
-      <c r="B5" s="98" t="s">
+      <c r="B5" s="100" t="s">
         <v>145</v>
       </c>
-      <c r="C5" s="98"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="98"/>
-      <c r="F5" s="98"/>
-      <c r="G5" s="98"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
@@ -8056,14 +8641,14 @@
       <c r="A6" s="71">
         <v>1</v>
       </c>
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="100" t="s">
         <v>146</v>
       </c>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="98"/>
-      <c r="G6" s="98"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="100"/>
+      <c r="F6" s="100"/>
+      <c r="G6" s="100"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>

</xml_diff>

<commit_message>
max pts testing complete
</commit_message>
<xml_diff>
--- a/excel-docs/euro - lifecycle info.xlsx
+++ b/excel-docs/euro - lifecycle info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joseph.collins/Documents/personal-projects/euro/2024_euro/excel-docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42A7C16-D948-8F45-AA27-A116157BA303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B64B124-D620-D544-A5CC-37E56C09082A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18000" yWindow="760" windowWidth="16560" windowHeight="20120" firstSheet="4" activeTab="6" xr2:uid="{D89656BD-B983-D041-A997-C1184058734E}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="20480" windowHeight="20120" firstSheet="4" activeTab="7" xr2:uid="{D89656BD-B983-D041-A997-C1184058734E}"/>
   </bookViews>
   <sheets>
     <sheet name="life cycle actions" sheetId="6" r:id="rId1"/>
@@ -1499,6 +1499,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1510,10 +1514,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2689,7 +2689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08564AC3-4506-8F41-9905-B73B2E25376A}">
   <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView topLeftCell="K17" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
@@ -2717,14 +2717,14 @@
       <c r="A2" s="70">
         <v>5</v>
       </c>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="112" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
       <c r="H2" s="66">
         <v>5</v>
       </c>
@@ -2733,14 +2733,14 @@
       <c r="A3" s="78">
         <v>4</v>
       </c>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="112" t="s">
         <v>142</v>
       </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
       <c r="H3" s="66">
         <v>4</v>
       </c>
@@ -2749,14 +2749,14 @@
       <c r="A4" s="73">
         <v>3</v>
       </c>
-      <c r="B4" s="115" t="s">
+      <c r="B4" s="112" t="s">
         <v>144</v>
       </c>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
       <c r="H4" s="66">
         <v>3</v>
       </c>
@@ -2765,14 +2765,14 @@
       <c r="A5" s="79">
         <v>2</v>
       </c>
-      <c r="B5" s="115" t="s">
+      <c r="B5" s="112" t="s">
         <v>145</v>
       </c>
-      <c r="C5" s="115"/>
-      <c r="D5" s="115"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="115"/>
-      <c r="G5" s="115"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
       <c r="H5" s="66">
         <v>2</v>
       </c>
@@ -2781,14 +2781,14 @@
       <c r="A6" s="71">
         <v>1</v>
       </c>
-      <c r="B6" s="115" t="s">
+      <c r="B6" s="112" t="s">
         <v>146</v>
       </c>
-      <c r="C6" s="115"/>
-      <c r="D6" s="115"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="115"/>
-      <c r="G6" s="115"/>
+      <c r="C6" s="112"/>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="112"/>
+      <c r="G6" s="112"/>
       <c r="H6" s="66">
         <v>1</v>
       </c>
@@ -3608,19 +3608,19 @@
       <c r="K41" s="64"/>
     </row>
     <row r="42" spans="9:20" x14ac:dyDescent="0.2">
-      <c r="J42" s="114" t="s">
+      <c r="J42" s="116" t="s">
         <v>255</v>
       </c>
-      <c r="K42" s="114"/>
-      <c r="L42" s="114"/>
-      <c r="M42" s="114"/>
-      <c r="N42" s="114"/>
-      <c r="O42" s="114"/>
-      <c r="P42" s="114"/>
-      <c r="Q42" s="114"/>
-      <c r="R42" s="114"/>
-      <c r="S42" s="114"/>
-      <c r="T42" s="114"/>
+      <c r="K42" s="116"/>
+      <c r="L42" s="116"/>
+      <c r="M42" s="116"/>
+      <c r="N42" s="116"/>
+      <c r="O42" s="116"/>
+      <c r="P42" s="116"/>
+      <c r="Q42" s="116"/>
+      <c r="R42" s="116"/>
+      <c r="S42" s="116"/>
+      <c r="T42" s="116"/>
     </row>
     <row r="43" spans="9:20" x14ac:dyDescent="0.2">
       <c r="J43" s="66" t="s">
@@ -3677,11 +3677,11 @@
         <f>IF(L44=L31,2,0)</f>
         <v>0</v>
       </c>
-      <c r="M45" s="111" t="str">
+      <c r="M45" s="113" t="str">
         <f>master!G27</f>
         <v>england</v>
       </c>
-      <c r="Q45" s="111" t="str">
+      <c r="Q45" s="113" t="str">
         <f>master!K27</f>
         <v>france</v>
       </c>
@@ -3702,7 +3702,7 @@
       <c r="L46" s="65" t="s">
         <v>235</v>
       </c>
-      <c r="M46" s="112"/>
+      <c r="M46" s="114"/>
       <c r="O46" s="65" t="s">
         <v>152</v>
       </c>
@@ -3849,11 +3849,11 @@
         <f>IF(L50=L37,2,0)</f>
         <v>2</v>
       </c>
-      <c r="M51" s="111" t="str">
+      <c r="M51" s="113" t="str">
         <f>master!G33</f>
         <v>spain</v>
       </c>
-      <c r="Q51" s="111" t="str">
+      <c r="Q51" s="113" t="str">
         <f>master!K33</f>
         <v>usa</v>
       </c>
@@ -3874,7 +3874,7 @@
       <c r="L52" s="65" t="s">
         <v>237</v>
       </c>
-      <c r="M52" s="112"/>
+      <c r="M52" s="114"/>
       <c r="Q52" s="119"/>
       <c r="R52" s="65" t="s">
         <v>241</v>
@@ -3966,11 +3966,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
     <mergeCell ref="M51:M52"/>
     <mergeCell ref="Q51:Q52"/>
     <mergeCell ref="M32:M33"/>
@@ -3978,6 +3973,11 @@
     <mergeCell ref="J42:T42"/>
     <mergeCell ref="M45:M46"/>
     <mergeCell ref="Q45:Q46"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <conditionalFormatting sqref="H10 N10 H17 N17 H24 N24">
     <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
@@ -4032,8 +4032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EC49F1C-9819-6A4D-BA8A-D847526C8B5C}">
   <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView topLeftCell="J11" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42:T42"/>
+    <sheetView topLeftCell="G10" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q9:Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4060,14 +4060,14 @@
       <c r="A2" s="70">
         <v>5</v>
       </c>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="112" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
       <c r="H2" s="66">
         <v>5</v>
       </c>
@@ -4076,14 +4076,14 @@
       <c r="A3" s="78">
         <v>4</v>
       </c>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="112" t="s">
         <v>142</v>
       </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
       <c r="H3" s="66">
         <v>4</v>
       </c>
@@ -4092,14 +4092,14 @@
       <c r="A4" s="73">
         <v>3</v>
       </c>
-      <c r="B4" s="115" t="s">
+      <c r="B4" s="112" t="s">
         <v>144</v>
       </c>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
       <c r="H4" s="66">
         <v>3</v>
       </c>
@@ -4108,14 +4108,14 @@
       <c r="A5" s="79">
         <v>2</v>
       </c>
-      <c r="B5" s="115" t="s">
+      <c r="B5" s="112" t="s">
         <v>145</v>
       </c>
-      <c r="C5" s="115"/>
-      <c r="D5" s="115"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="115"/>
-      <c r="G5" s="115"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
       <c r="H5" s="66">
         <v>2</v>
       </c>
@@ -4124,14 +4124,14 @@
       <c r="A6" s="71">
         <v>1</v>
       </c>
-      <c r="B6" s="115" t="s">
+      <c r="B6" s="112" t="s">
         <v>146</v>
       </c>
-      <c r="C6" s="115"/>
-      <c r="D6" s="115"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="115"/>
-      <c r="G6" s="115"/>
+      <c r="C6" s="112"/>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="112"/>
+      <c r="G6" s="112"/>
       <c r="H6" s="66">
         <v>1</v>
       </c>
@@ -4951,19 +4951,19 @@
       <c r="K41" s="64"/>
     </row>
     <row r="42" spans="9:20" x14ac:dyDescent="0.2">
-      <c r="J42" s="114" t="s">
+      <c r="J42" s="116" t="s">
         <v>255</v>
       </c>
-      <c r="K42" s="114"/>
-      <c r="L42" s="114"/>
-      <c r="M42" s="114"/>
-      <c r="N42" s="114"/>
-      <c r="O42" s="114"/>
-      <c r="P42" s="114"/>
-      <c r="Q42" s="114"/>
-      <c r="R42" s="114"/>
-      <c r="S42" s="114"/>
-      <c r="T42" s="114"/>
+      <c r="K42" s="116"/>
+      <c r="L42" s="116"/>
+      <c r="M42" s="116"/>
+      <c r="N42" s="116"/>
+      <c r="O42" s="116"/>
+      <c r="P42" s="116"/>
+      <c r="Q42" s="116"/>
+      <c r="R42" s="116"/>
+      <c r="S42" s="116"/>
+      <c r="T42" s="116"/>
     </row>
     <row r="43" spans="9:20" x14ac:dyDescent="0.2">
       <c r="J43" s="66" t="s">
@@ -5020,11 +5020,11 @@
         <f>IF(L44=L31,2,0)</f>
         <v>2</v>
       </c>
-      <c r="M45" s="111" t="str">
+      <c r="M45" s="113" t="str">
         <f>master!G27</f>
         <v>england</v>
       </c>
-      <c r="Q45" s="111" t="str">
+      <c r="Q45" s="113" t="str">
         <f>master!K27</f>
         <v>france</v>
       </c>
@@ -5045,7 +5045,7 @@
       <c r="L46" s="65" t="s">
         <v>235</v>
       </c>
-      <c r="M46" s="112"/>
+      <c r="M46" s="114"/>
       <c r="O46" s="65" t="s">
         <v>152</v>
       </c>
@@ -5192,11 +5192,11 @@
         <f>IF(L50=L37,2,0)</f>
         <v>0</v>
       </c>
-      <c r="M51" s="111" t="str">
+      <c r="M51" s="113" t="str">
         <f>master!G33</f>
         <v>spain</v>
       </c>
-      <c r="Q51" s="111" t="str">
+      <c r="Q51" s="113" t="str">
         <f>master!K33</f>
         <v>usa</v>
       </c>
@@ -5217,7 +5217,7 @@
       <c r="L52" s="65" t="s">
         <v>237</v>
       </c>
-      <c r="M52" s="112"/>
+      <c r="M52" s="114"/>
       <c r="Q52" s="119"/>
       <c r="R52" s="65" t="s">
         <v>241</v>
@@ -5309,11 +5309,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
     <mergeCell ref="M51:M52"/>
     <mergeCell ref="Q51:Q52"/>
     <mergeCell ref="M32:M33"/>
@@ -5321,6 +5316,11 @@
     <mergeCell ref="J42:T42"/>
     <mergeCell ref="M45:M46"/>
     <mergeCell ref="Q45:Q46"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <conditionalFormatting sqref="H10 N10 H17 N17 H24 N24">
     <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
@@ -5392,15 +5392,15 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="114" t="s">
+      <c r="A2" s="116" t="s">
         <v>229</v>
       </c>
-      <c r="B2" s="114"/>
-      <c r="C2" s="114"/>
-      <c r="D2" s="114"/>
-      <c r="E2" s="114"/>
-      <c r="F2" s="114"/>
-      <c r="G2" s="114"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="122" t="s">
@@ -5576,15 +5576,15 @@
       <c r="G13" s="121"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="114" t="s">
+      <c r="A16" s="116" t="s">
         <v>242</v>
       </c>
-      <c r="B16" s="114"/>
-      <c r="C16" s="114"/>
-      <c r="D16" s="114"/>
-      <c r="E16" s="114"/>
-      <c r="F16" s="114"/>
-      <c r="G16" s="114"/>
+      <c r="B16" s="116"/>
+      <c r="C16" s="116"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="116"/>
+      <c r="G16" s="116"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="120" t="s">
@@ -5761,6 +5761,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A20:A21"/>
@@ -5777,8 +5779,6 @@
     <mergeCell ref="A16:G16"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7027,8 +7027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F2D8727-69E7-4348-A9F0-3DA347775291}">
   <dimension ref="A1:AE57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C12" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Y10" sqref="Y10:Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7057,14 +7057,14 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="68"/>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="112" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
@@ -7075,14 +7075,14 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="77"/>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="112" t="s">
         <v>142</v>
       </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
@@ -7093,14 +7093,14 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="72"/>
-      <c r="B4" s="115" t="s">
+      <c r="B4" s="112" t="s">
         <v>144</v>
       </c>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
@@ -7111,14 +7111,14 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="69"/>
-      <c r="B5" s="115" t="s">
+      <c r="B5" s="112" t="s">
         <v>145</v>
       </c>
-      <c r="C5" s="115"/>
-      <c r="D5" s="115"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="115"/>
-      <c r="G5" s="115"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
@@ -7129,14 +7129,14 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="22"/>
-      <c r="B6" s="115" t="s">
+      <c r="B6" s="112" t="s">
         <v>146</v>
       </c>
-      <c r="C6" s="115"/>
-      <c r="D6" s="115"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="115"/>
-      <c r="G6" s="115"/>
+      <c r="C6" s="112"/>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="112"/>
+      <c r="G6" s="112"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
@@ -8047,7 +8047,7 @@
       <c r="AE30" s="89"/>
     </row>
     <row r="31" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C31" s="116"/>
+      <c r="C31" s="111"/>
       <c r="D31" s="66" t="s">
         <v>211</v>
       </c>
@@ -8069,7 +8069,7 @@
       </c>
     </row>
     <row r="32" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C32" s="116"/>
+      <c r="C32" s="111"/>
       <c r="D32" s="76" t="s">
         <v>221</v>
       </c>
@@ -8114,7 +8114,7 @@
       <c r="AE33" s="89"/>
     </row>
     <row r="34" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C34" s="116"/>
+      <c r="C34" s="111"/>
       <c r="D34" s="70" t="s">
         <v>212</v>
       </c>
@@ -8141,7 +8141,7 @@
       </c>
     </row>
     <row r="35" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C35" s="116"/>
+      <c r="C35" s="111"/>
       <c r="D35" s="70" t="s">
         <v>217</v>
       </c>
@@ -8188,7 +8188,7 @@
       <c r="AE36" s="89"/>
     </row>
     <row r="37" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C37" s="116"/>
+      <c r="C37" s="111"/>
       <c r="D37" s="66" t="s">
         <v>225</v>
       </c>
@@ -8211,7 +8211,7 @@
       </c>
     </row>
     <row r="38" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C38" s="116"/>
+      <c r="C38" s="111"/>
       <c r="D38" s="76" t="s">
         <v>256</v>
       </c>
@@ -8236,7 +8236,7 @@
       <c r="X38" s="76" t="s">
         <v>227</v>
       </c>
-      <c r="AE38" s="116"/>
+      <c r="AE38" s="111"/>
     </row>
     <row r="39" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C39"/>
@@ -8250,10 +8250,10 @@
       </c>
       <c r="W39" s="66"/>
       <c r="X39" s="66"/>
-      <c r="AE39" s="116"/>
+      <c r="AE39" s="111"/>
     </row>
     <row r="40" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C40" s="116"/>
+      <c r="C40" s="111"/>
       <c r="D40" s="70" t="s">
         <v>220</v>
       </c>
@@ -8276,7 +8276,7 @@
       </c>
     </row>
     <row r="41" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C41" s="116"/>
+      <c r="C41" s="111"/>
       <c r="D41" s="70" t="s">
         <v>223</v>
       </c>
@@ -8297,29 +8297,29 @@
       </c>
     </row>
     <row r="43" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="D43" s="114" t="s">
+      <c r="D43" s="116" t="s">
         <v>255</v>
       </c>
-      <c r="E43" s="114"/>
-      <c r="F43" s="114"/>
-      <c r="G43" s="114"/>
-      <c r="H43" s="114"/>
-      <c r="I43" s="114"/>
-      <c r="J43" s="114"/>
-      <c r="K43" s="114"/>
-      <c r="L43" s="114"/>
-      <c r="M43" s="114"/>
-      <c r="N43" s="114"/>
-      <c r="O43" s="114"/>
-      <c r="P43" s="114"/>
-      <c r="Q43" s="114"/>
-      <c r="R43" s="114"/>
-      <c r="S43" s="114"/>
-      <c r="T43" s="114"/>
-      <c r="U43" s="114"/>
-      <c r="V43" s="114"/>
-      <c r="W43" s="114"/>
-      <c r="X43" s="114"/>
+      <c r="E43" s="116"/>
+      <c r="F43" s="116"/>
+      <c r="G43" s="116"/>
+      <c r="H43" s="116"/>
+      <c r="I43" s="116"/>
+      <c r="J43" s="116"/>
+      <c r="K43" s="116"/>
+      <c r="L43" s="116"/>
+      <c r="M43" s="116"/>
+      <c r="N43" s="116"/>
+      <c r="O43" s="116"/>
+      <c r="P43" s="116"/>
+      <c r="Q43" s="116"/>
+      <c r="R43" s="116"/>
+      <c r="S43" s="116"/>
+      <c r="T43" s="116"/>
+      <c r="U43" s="116"/>
+      <c r="V43" s="116"/>
+      <c r="W43" s="116"/>
+      <c r="X43" s="116"/>
     </row>
     <row r="44" spans="3:31" x14ac:dyDescent="0.2">
       <c r="D44" s="66" t="s">
@@ -8378,12 +8378,12 @@
         <f>IF(F45=F32,2,0)</f>
         <v>2</v>
       </c>
-      <c r="G46" s="111" t="str">
+      <c r="G46" s="113" t="str">
         <f>master!G27</f>
         <v>england</v>
       </c>
       <c r="M46" s="64"/>
-      <c r="P46" s="113" t="str">
+      <c r="P46" s="115" t="str">
         <f>master!K27</f>
         <v>france</v>
       </c>
@@ -8404,12 +8404,12 @@
       <c r="F47" s="65" t="s">
         <v>235</v>
       </c>
-      <c r="G47" s="112"/>
+      <c r="G47" s="114"/>
       <c r="M47" s="67"/>
       <c r="N47" s="65" t="s">
         <v>152</v>
       </c>
-      <c r="P47" s="113"/>
+      <c r="P47" s="115"/>
       <c r="V47" s="90" t="s">
         <v>239</v>
       </c>
@@ -8438,7 +8438,7 @@
       <c r="L48" s="65" t="s">
         <v>225</v>
       </c>
-      <c r="N48" s="113" t="str">
+      <c r="N48" s="115" t="str">
         <f>master!I29</f>
         <v>france</v>
       </c>
@@ -8467,12 +8467,12 @@
         <f>IF(F48=F35,2,0)</f>
         <v>2</v>
       </c>
-      <c r="L49" s="113" t="str">
+      <c r="L49" s="115" t="str">
         <f>master!H30</f>
         <v>england</v>
       </c>
-      <c r="N49" s="113"/>
-      <c r="O49" s="113" t="str">
+      <c r="N49" s="115"/>
+      <c r="O49" s="115" t="str">
         <f>master!J30</f>
         <v>france</v>
       </c>
@@ -8493,12 +8493,12 @@
       <c r="F50" s="65" t="s">
         <v>236</v>
       </c>
-      <c r="L50" s="113"/>
+      <c r="L50" s="115"/>
       <c r="N50" s="64">
         <f>IF(N48=N35,10,0)</f>
         <v>10</v>
       </c>
-      <c r="O50" s="113"/>
+      <c r="O50" s="115"/>
       <c r="V50" s="65" t="s">
         <v>240</v>
       </c>
@@ -8551,11 +8551,11 @@
         <f>IF(F51=F38,2,0)</f>
         <v>2</v>
       </c>
-      <c r="G52" s="111" t="str">
+      <c r="G52" s="113" t="str">
         <f>master!G33</f>
         <v>spain</v>
       </c>
-      <c r="P52" s="113" t="str">
+      <c r="P52" s="115" t="str">
         <f>master!K33</f>
         <v>usa</v>
       </c>
@@ -8576,8 +8576,8 @@
       <c r="F53" s="65" t="s">
         <v>237</v>
       </c>
-      <c r="G53" s="112"/>
-      <c r="P53" s="113"/>
+      <c r="G53" s="114"/>
+      <c r="P53" s="115"/>
       <c r="V53" s="65" t="s">
         <v>241</v>
       </c>
@@ -8697,6 +8697,19 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="P52:P53"/>
+    <mergeCell ref="D43:X43"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="P46:P47"/>
+    <mergeCell ref="N48:N49"/>
+    <mergeCell ref="L49:L50"/>
+    <mergeCell ref="O49:O50"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="AE38:AE39"/>
     <mergeCell ref="G39:G40"/>
@@ -8709,19 +8722,6 @@
     <mergeCell ref="L36:L37"/>
     <mergeCell ref="O36:O37"/>
     <mergeCell ref="N35:N36"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="P52:P53"/>
-    <mergeCell ref="D43:X43"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="P46:P47"/>
-    <mergeCell ref="N48:N49"/>
-    <mergeCell ref="L49:L50"/>
-    <mergeCell ref="O49:O50"/>
   </mergeCells>
   <conditionalFormatting sqref="L10 V10 L17 V17 L24 V24">
     <cfRule type="cellIs" dxfId="32" priority="6" operator="equal">
@@ -8754,8 +8754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02BA53A3-896F-5548-BE26-1B0315E4CCCA}">
   <dimension ref="A1:AD56"/>
   <sheetViews>
-    <sheetView topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView tabSelected="1" topLeftCell="H12" workbookViewId="0">
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8783,14 +8783,14 @@
       <c r="A2" s="70">
         <v>5</v>
       </c>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="112" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
       <c r="H2" s="66">
         <v>5</v>
       </c>
@@ -8799,14 +8799,14 @@
       <c r="A3" s="78">
         <v>4</v>
       </c>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="112" t="s">
         <v>142</v>
       </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
       <c r="H3" s="66">
         <v>4</v>
       </c>
@@ -8815,14 +8815,14 @@
       <c r="A4" s="73">
         <v>3</v>
       </c>
-      <c r="B4" s="115" t="s">
+      <c r="B4" s="112" t="s">
         <v>144</v>
       </c>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
       <c r="H4" s="66">
         <v>3</v>
       </c>
@@ -8831,14 +8831,14 @@
       <c r="A5" s="79">
         <v>2</v>
       </c>
-      <c r="B5" s="115" t="s">
+      <c r="B5" s="112" t="s">
         <v>145</v>
       </c>
-      <c r="C5" s="115"/>
-      <c r="D5" s="115"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="115"/>
-      <c r="G5" s="115"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
       <c r="H5" s="66">
         <v>2</v>
       </c>
@@ -8847,14 +8847,14 @@
       <c r="A6" s="71">
         <v>1</v>
       </c>
-      <c r="B6" s="115" t="s">
+      <c r="B6" s="112" t="s">
         <v>146</v>
       </c>
-      <c r="C6" s="115"/>
-      <c r="D6" s="115"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="115"/>
-      <c r="G6" s="115"/>
+      <c r="C6" s="112"/>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="112"/>
+      <c r="G6" s="112"/>
       <c r="H6" s="66">
         <v>1</v>
       </c>
@@ -9161,6 +9161,9 @@
       </c>
       <c r="O18" s="64"/>
       <c r="P18" s="64"/>
+      <c r="Q18">
+        <v>72</v>
+      </c>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D19" s="66" t="s">
@@ -9195,6 +9198,9 @@
       </c>
       <c r="O19" s="64"/>
       <c r="P19" s="64"/>
+      <c r="Q19">
+        <v>6</v>
+      </c>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D20" s="66" t="s">
@@ -9688,19 +9694,19 @@
       <c r="K41" s="64"/>
     </row>
     <row r="42" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="J42" s="114" t="s">
+      <c r="J42" s="116" t="s">
         <v>255</v>
       </c>
-      <c r="K42" s="114"/>
-      <c r="L42" s="114"/>
-      <c r="M42" s="114"/>
-      <c r="N42" s="114"/>
-      <c r="O42" s="114"/>
-      <c r="P42" s="114"/>
-      <c r="Q42" s="114"/>
-      <c r="R42" s="114"/>
-      <c r="S42" s="114"/>
-      <c r="T42" s="114"/>
+      <c r="K42" s="116"/>
+      <c r="L42" s="116"/>
+      <c r="M42" s="116"/>
+      <c r="N42" s="116"/>
+      <c r="O42" s="116"/>
+      <c r="P42" s="116"/>
+      <c r="Q42" s="116"/>
+      <c r="R42" s="116"/>
+      <c r="S42" s="116"/>
+      <c r="T42" s="116"/>
       <c r="U42" s="80"/>
       <c r="V42" s="80"/>
       <c r="W42" s="80"/>
@@ -9767,11 +9773,11 @@
         <f>IF(L44=L31,2,0)</f>
         <v>0</v>
       </c>
-      <c r="M45" s="111" t="str">
+      <c r="M45" s="113" t="str">
         <f>master!G27</f>
         <v>england</v>
       </c>
-      <c r="Q45" s="111" t="str">
+      <c r="Q45" s="113" t="str">
         <f>master!K27</f>
         <v>france</v>
       </c>
@@ -9792,7 +9798,7 @@
       <c r="L46" s="65" t="s">
         <v>235</v>
       </c>
-      <c r="M46" s="112"/>
+      <c r="M46" s="114"/>
       <c r="O46" s="65" t="s">
         <v>152</v>
       </c>
@@ -9939,11 +9945,11 @@
         <f>IF(L50=L37,2,0)</f>
         <v>2</v>
       </c>
-      <c r="M51" s="111" t="str">
+      <c r="M51" s="113" t="str">
         <f>master!G33</f>
         <v>spain</v>
       </c>
-      <c r="Q51" s="111" t="str">
+      <c r="Q51" s="113" t="str">
         <f>master!K33</f>
         <v>usa</v>
       </c>
@@ -9964,7 +9970,7 @@
       <c r="L52" s="65" t="s">
         <v>237</v>
       </c>
-      <c r="M52" s="112"/>
+      <c r="M52" s="114"/>
       <c r="Q52" s="119"/>
       <c r="R52" s="65" t="s">
         <v>241</v>
@@ -10058,6 +10064,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="M51:M52"/>
+    <mergeCell ref="J42:T42"/>
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="M45:M46"/>
+    <mergeCell ref="Q51:Q52"/>
     <mergeCell ref="M32:M33"/>
     <mergeCell ref="Q45:Q46"/>
     <mergeCell ref="B2:G2"/>
@@ -10065,11 +10076,6 @@
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B5:G5"/>
     <mergeCell ref="B6:G6"/>
-    <mergeCell ref="M51:M52"/>
-    <mergeCell ref="J42:T42"/>
-    <mergeCell ref="M38:M39"/>
-    <mergeCell ref="M45:M46"/>
-    <mergeCell ref="Q51:Q52"/>
   </mergeCells>
   <conditionalFormatting sqref="H10 M10 H17 M17 H24 M24">
     <cfRule type="cellIs" dxfId="27" priority="14" operator="equal">
@@ -10124,7 +10130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3292362C-0E51-2145-8D28-B6F8E9B96320}">
   <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView topLeftCell="G14" workbookViewId="0">
+    <sheetView topLeftCell="E7" workbookViewId="0">
       <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
@@ -10152,14 +10158,14 @@
       <c r="A2" s="70">
         <v>5</v>
       </c>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="112" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
       <c r="H2" s="66">
         <v>5</v>
       </c>
@@ -10168,14 +10174,14 @@
       <c r="A3" s="78">
         <v>4</v>
       </c>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="112" t="s">
         <v>142</v>
       </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
       <c r="H3" s="66">
         <v>4</v>
       </c>
@@ -10184,14 +10190,14 @@
       <c r="A4" s="73">
         <v>3</v>
       </c>
-      <c r="B4" s="115" t="s">
+      <c r="B4" s="112" t="s">
         <v>144</v>
       </c>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
       <c r="H4" s="66">
         <v>3</v>
       </c>
@@ -10200,14 +10206,14 @@
       <c r="A5" s="79">
         <v>2</v>
       </c>
-      <c r="B5" s="115" t="s">
+      <c r="B5" s="112" t="s">
         <v>145</v>
       </c>
-      <c r="C5" s="115"/>
-      <c r="D5" s="115"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="115"/>
-      <c r="G5" s="115"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
       <c r="H5" s="66">
         <v>2</v>
       </c>
@@ -10216,14 +10222,14 @@
       <c r="A6" s="71">
         <v>1</v>
       </c>
-      <c r="B6" s="115" t="s">
+      <c r="B6" s="112" t="s">
         <v>146</v>
       </c>
-      <c r="C6" s="115"/>
-      <c r="D6" s="115"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="115"/>
-      <c r="G6" s="115"/>
+      <c r="C6" s="112"/>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="112"/>
+      <c r="G6" s="112"/>
       <c r="H6" s="66">
         <v>1</v>
       </c>
@@ -11043,19 +11049,19 @@
       <c r="K41" s="64"/>
     </row>
     <row r="42" spans="9:20" x14ac:dyDescent="0.2">
-      <c r="J42" s="114" t="s">
+      <c r="J42" s="116" t="s">
         <v>255</v>
       </c>
-      <c r="K42" s="114"/>
-      <c r="L42" s="114"/>
-      <c r="M42" s="114"/>
-      <c r="N42" s="114"/>
-      <c r="O42" s="114"/>
-      <c r="P42" s="114"/>
-      <c r="Q42" s="114"/>
-      <c r="R42" s="114"/>
-      <c r="S42" s="114"/>
-      <c r="T42" s="114"/>
+      <c r="K42" s="116"/>
+      <c r="L42" s="116"/>
+      <c r="M42" s="116"/>
+      <c r="N42" s="116"/>
+      <c r="O42" s="116"/>
+      <c r="P42" s="116"/>
+      <c r="Q42" s="116"/>
+      <c r="R42" s="116"/>
+      <c r="S42" s="116"/>
+      <c r="T42" s="116"/>
     </row>
     <row r="43" spans="9:20" x14ac:dyDescent="0.2">
       <c r="J43" s="66" t="s">
@@ -11112,11 +11118,11 @@
         <f>IF(L44=L31,2,0)</f>
         <v>2</v>
       </c>
-      <c r="M45" s="111" t="str">
+      <c r="M45" s="113" t="str">
         <f>master!G27</f>
         <v>england</v>
       </c>
-      <c r="Q45" s="111" t="str">
+      <c r="Q45" s="113" t="str">
         <f>master!K27</f>
         <v>france</v>
       </c>
@@ -11137,7 +11143,7 @@
       <c r="L46" s="65" t="s">
         <v>235</v>
       </c>
-      <c r="M46" s="112"/>
+      <c r="M46" s="114"/>
       <c r="O46" s="65" t="s">
         <v>152</v>
       </c>
@@ -11284,11 +11290,11 @@
         <f>IF(L50=L37,2,0)</f>
         <v>0</v>
       </c>
-      <c r="M51" s="111" t="str">
+      <c r="M51" s="113" t="str">
         <f>master!G33</f>
         <v>spain</v>
       </c>
-      <c r="Q51" s="111" t="str">
+      <c r="Q51" s="113" t="str">
         <f>master!K33</f>
         <v>usa</v>
       </c>
@@ -11309,7 +11315,7 @@
       <c r="L52" s="65" t="s">
         <v>237</v>
       </c>
-      <c r="M52" s="112"/>
+      <c r="M52" s="114"/>
       <c r="Q52" s="119"/>
       <c r="R52" s="65" t="s">
         <v>241</v>
@@ -11401,11 +11407,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
     <mergeCell ref="M51:M52"/>
     <mergeCell ref="Q51:Q52"/>
     <mergeCell ref="M32:M33"/>
@@ -11413,6 +11414,11 @@
     <mergeCell ref="J42:T42"/>
     <mergeCell ref="M45:M46"/>
     <mergeCell ref="Q45:Q46"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <conditionalFormatting sqref="H10 N10 H17 N17 H24 N24">
     <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">

</xml_diff>

<commit_message>
last updated and payout work for mobile view started
</commit_message>
<xml_diff>
--- a/excel-docs/euro - lifecycle info.xlsx
+++ b/excel-docs/euro - lifecycle info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joseph.collins/Documents/personal-projects/euro/2024_euro/excel-docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD20B6C2-7083-A445-BB72-8F2FC141BDD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0AB45F-82EE-8342-8B7D-A5ED308EC1B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34560" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D89656BD-B983-D041-A997-C1184058734E}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1291" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="258">
   <si>
     <t>need to submit a number for tiebreaker score</t>
   </si>
@@ -914,6 +914,9 @@
 KO stages
 -comp view
 -mobile view</t>
+  </si>
+  <si>
+    <t>Header &gt; Misc Header Data --- bring in the loadUsersWhoNeedWebsiteUpdatedEmails func</t>
   </si>
 </sst>
 </file>
@@ -1507,6 +1510,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1518,10 +1525,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2097,7 +2100,7 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:F106"/>
+  <dimension ref="A1:F107"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -2149,545 +2152,551 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="99"/>
+      <c r="A6" s="98"/>
       <c r="B6" s="32" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="99"/>
+      <c r="B7" s="32" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="15"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="95">
+    <row r="8" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="15"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="95">
         <v>2</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B9" s="32" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="96"/>
-      <c r="B9" s="33" t="s">
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="96"/>
+      <c r="B10" s="33" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-    </row>
-    <row r="11" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="94">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="6"/>
+      <c r="B11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="94">
         <v>3</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B12" s="10" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="24" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="94"/>
-      <c r="B12" s="23" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="94"/>
       <c r="B13" s="23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="24" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="94"/>
+      <c r="B14" s="23" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="94"/>
-      <c r="B14" s="34" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="94"/>
       <c r="B15" s="34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="94"/>
       <c r="B16" s="34" t="s">
-        <v>61</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="94"/>
       <c r="B17" s="34" t="s">
-        <v>95</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="94"/>
       <c r="B18" s="34" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="94"/>
       <c r="B19" s="34" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="94"/>
       <c r="B20" s="34" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="94"/>
       <c r="B21" s="34" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="94"/>
       <c r="B22" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="94"/>
       <c r="B23" s="34" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="94"/>
       <c r="B24" s="34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="94"/>
+      <c r="B25" s="34" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="6"/>
-      <c r="B25" s="7"/>
-    </row>
-    <row r="26" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A26" s="94">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="6"/>
+      <c r="B26" s="7"/>
+    </row>
+    <row r="27" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A27" s="94">
         <v>4</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B27" s="10" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="24" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="94"/>
-      <c r="B27" s="23" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="94"/>
       <c r="B28" s="23" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="24" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="94"/>
+      <c r="B29" s="23" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="94"/>
-      <c r="B29" s="21" t="s">
+    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="94"/>
+      <c r="B30" s="21" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="94"/>
-      <c r="B30" s="34" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="94"/>
       <c r="B31" s="34" t="s">
-        <v>95</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="94"/>
       <c r="B32" s="34" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="94"/>
       <c r="B33" s="34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="94"/>
       <c r="B34" s="34" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="94"/>
       <c r="B35" s="34" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="94"/>
       <c r="B36" s="34" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="94"/>
+      <c r="B37" s="34" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="6"/>
-      <c r="B37" s="7"/>
-    </row>
-    <row r="38" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="B38" s="10" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="6"/>
+      <c r="B38" s="7"/>
+    </row>
+    <row r="39" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="B39" s="10" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B39" s="32" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B40" s="32" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B41" s="32" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B42" s="32" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="25" t="s">
+    <row r="43" spans="1:2" ht="21" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="25" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="24" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="23" t="s">
+    <row r="44" spans="1:2" ht="24" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="23" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="24" x14ac:dyDescent="0.3">
-      <c r="B44" s="38" t="s">
+    <row r="45" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="B45" s="38" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B45" s="32" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B46" s="32" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B46" s="34" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B47" s="34" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B47" s="36" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B48" s="36" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B48" s="34" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B49" s="34" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B50" s="34" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B50" s="37" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B51" s="37" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B51" s="34" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B52" s="34" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B53" s="34" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B54" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C53" s="9"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="6"/>
-      <c r="B54" s="7"/>
-    </row>
-    <row r="55" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="B55" s="10" t="s">
+      <c r="C54" s="9"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="6"/>
+      <c r="B55" s="7"/>
+    </row>
+    <row r="56" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="B56" s="10" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B56" s="21" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B57" s="21" t="s">
-        <v>105</v>
+        <v>68</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B58" s="21" t="s">
-        <v>37</v>
+        <v>105</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B59" s="21" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B60" s="21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B61" s="21" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B61" s="24" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B62" s="24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B62" s="26" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B63" s="26" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B63" s="24" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B64" s="24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B65" s="24" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B65" s="27" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B66" s="27" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B66" s="22" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B67" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B68" s="22" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B68" s="24" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B69" s="24" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" s="6"/>
-      <c r="B69" s="7"/>
-    </row>
-    <row r="70" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="B70" s="10" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="6"/>
+      <c r="B70" s="7"/>
+    </row>
+    <row r="71" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="B71" s="10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B71" s="21" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B72" s="21" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="24" x14ac:dyDescent="0.3">
-      <c r="B72" s="23" t="s">
+    <row r="73" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="B73" s="23" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="31" t="s">
+    <row r="74" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="31" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B74" s="21" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B75" s="21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B76" s="21" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B76" s="24" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B77" s="24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B77" s="26" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B78" s="26" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B78" s="24" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B79" s="24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B80" s="24" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B80" s="27" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B81" s="27" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B81" s="22" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B82" s="22" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B83" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B84" s="22" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B85" s="22" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B86" s="22" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B86" s="24" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B87" s="24" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="6"/>
-      <c r="B87" s="7"/>
-    </row>
-    <row r="88" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="B88" s="10" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="6"/>
+      <c r="B88" s="7"/>
+    </row>
+    <row r="89" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="B89" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B89" s="21" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B90" s="21" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="24" x14ac:dyDescent="0.3">
-      <c r="B90" s="23" t="s">
+    <row r="91" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="B91" s="23" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B91" s="24" t="s">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B92" s="24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B92" s="26" t="s">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B93" s="26" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B93" s="24" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B94" s="24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B95" s="24" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B95" s="22" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B96" s="22" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B97" s="22" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B98" s="22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B99" s="22" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B99" s="24" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B100" s="24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B101" s="24" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" s="6"/>
-      <c r="B101" s="7"/>
-    </row>
-    <row r="102" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="B102" s="10" t="s">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="6"/>
+      <c r="B102" s="7"/>
+    </row>
+    <row r="103" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="B103" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="103" spans="1:2" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.3">
-      <c r="A103" s="29"/>
-      <c r="B103" s="23" t="s">
+    <row r="104" spans="1:2" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A104" s="29"/>
+      <c r="B104" s="23" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="104" spans="1:2" s="13" customFormat="1" ht="24" x14ac:dyDescent="0.3">
-      <c r="A104" s="30"/>
-      <c r="B104" s="23" t="s">
+    <row r="105" spans="1:2" s="13" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A105" s="30"/>
+      <c r="B105" s="23" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B105" s="21" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B106" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B107" s="21" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A11:A24"/>
-    <mergeCell ref="A26:A36"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A12:A25"/>
+    <mergeCell ref="A27:A37"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A2:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2725,14 +2734,14 @@
       <c r="A2" s="70">
         <v>5</v>
       </c>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="112" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
       <c r="H2" s="66">
         <v>5</v>
       </c>
@@ -2741,14 +2750,14 @@
       <c r="A3" s="78">
         <v>4</v>
       </c>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="112" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
       <c r="H3" s="66">
         <v>4</v>
       </c>
@@ -2757,14 +2766,14 @@
       <c r="A4" s="73">
         <v>3</v>
       </c>
-      <c r="B4" s="115" t="s">
+      <c r="B4" s="112" t="s">
         <v>143</v>
       </c>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
       <c r="H4" s="66">
         <v>3</v>
       </c>
@@ -2773,14 +2782,14 @@
       <c r="A5" s="79">
         <v>2</v>
       </c>
-      <c r="B5" s="115" t="s">
+      <c r="B5" s="112" t="s">
         <v>144</v>
       </c>
-      <c r="C5" s="115"/>
-      <c r="D5" s="115"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="115"/>
-      <c r="G5" s="115"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
       <c r="H5" s="66">
         <v>2</v>
       </c>
@@ -2789,14 +2798,14 @@
       <c r="A6" s="71">
         <v>1</v>
       </c>
-      <c r="B6" s="115" t="s">
+      <c r="B6" s="112" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="115"/>
-      <c r="D6" s="115"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="115"/>
-      <c r="G6" s="115"/>
+      <c r="C6" s="112"/>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="112"/>
+      <c r="G6" s="112"/>
       <c r="H6" s="66">
         <v>1</v>
       </c>
@@ -3616,19 +3625,19 @@
       <c r="K41" s="64"/>
     </row>
     <row r="42" spans="9:20" x14ac:dyDescent="0.2">
-      <c r="J42" s="114" t="s">
+      <c r="J42" s="116" t="s">
         <v>254</v>
       </c>
-      <c r="K42" s="114"/>
-      <c r="L42" s="114"/>
-      <c r="M42" s="114"/>
-      <c r="N42" s="114"/>
-      <c r="O42" s="114"/>
-      <c r="P42" s="114"/>
-      <c r="Q42" s="114"/>
-      <c r="R42" s="114"/>
-      <c r="S42" s="114"/>
-      <c r="T42" s="114"/>
+      <c r="K42" s="116"/>
+      <c r="L42" s="116"/>
+      <c r="M42" s="116"/>
+      <c r="N42" s="116"/>
+      <c r="O42" s="116"/>
+      <c r="P42" s="116"/>
+      <c r="Q42" s="116"/>
+      <c r="R42" s="116"/>
+      <c r="S42" s="116"/>
+      <c r="T42" s="116"/>
     </row>
     <row r="43" spans="9:20" x14ac:dyDescent="0.2">
       <c r="J43" s="66" t="s">
@@ -3685,11 +3694,11 @@
         <f>IF(L44=L31,2,0)</f>
         <v>0</v>
       </c>
-      <c r="M45" s="111" t="str">
+      <c r="M45" s="113" t="str">
         <f>master!G27</f>
         <v>england</v>
       </c>
-      <c r="Q45" s="111" t="str">
+      <c r="Q45" s="113" t="str">
         <f>master!K27</f>
         <v>france</v>
       </c>
@@ -3710,7 +3719,7 @@
       <c r="L46" s="65" t="s">
         <v>234</v>
       </c>
-      <c r="M46" s="112"/>
+      <c r="M46" s="114"/>
       <c r="O46" s="65" t="s">
         <v>151</v>
       </c>
@@ -3857,11 +3866,11 @@
         <f>IF(L50=L37,2,0)</f>
         <v>2</v>
       </c>
-      <c r="M51" s="111" t="str">
+      <c r="M51" s="113" t="str">
         <f>master!G33</f>
         <v>spain</v>
       </c>
-      <c r="Q51" s="111" t="str">
+      <c r="Q51" s="113" t="str">
         <f>master!K33</f>
         <v>usa</v>
       </c>
@@ -3882,7 +3891,7 @@
       <c r="L52" s="65" t="s">
         <v>236</v>
       </c>
-      <c r="M52" s="112"/>
+      <c r="M52" s="114"/>
       <c r="Q52" s="119"/>
       <c r="R52" s="65" t="s">
         <v>240</v>
@@ -3974,11 +3983,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
     <mergeCell ref="M51:M52"/>
     <mergeCell ref="Q51:Q52"/>
     <mergeCell ref="M32:M33"/>
@@ -3986,6 +3990,11 @@
     <mergeCell ref="J42:T42"/>
     <mergeCell ref="M45:M46"/>
     <mergeCell ref="Q45:Q46"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <conditionalFormatting sqref="H10 N10 H17 N17 H24 N24">
     <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
@@ -4068,14 +4077,14 @@
       <c r="A2" s="70">
         <v>5</v>
       </c>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="112" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
       <c r="H2" s="66">
         <v>5</v>
       </c>
@@ -4084,14 +4093,14 @@
       <c r="A3" s="78">
         <v>4</v>
       </c>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="112" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
       <c r="H3" s="66">
         <v>4</v>
       </c>
@@ -4100,14 +4109,14 @@
       <c r="A4" s="73">
         <v>3</v>
       </c>
-      <c r="B4" s="115" t="s">
+      <c r="B4" s="112" t="s">
         <v>143</v>
       </c>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
       <c r="H4" s="66">
         <v>3</v>
       </c>
@@ -4116,14 +4125,14 @@
       <c r="A5" s="79">
         <v>2</v>
       </c>
-      <c r="B5" s="115" t="s">
+      <c r="B5" s="112" t="s">
         <v>144</v>
       </c>
-      <c r="C5" s="115"/>
-      <c r="D5" s="115"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="115"/>
-      <c r="G5" s="115"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
       <c r="H5" s="66">
         <v>2</v>
       </c>
@@ -4132,14 +4141,14 @@
       <c r="A6" s="71">
         <v>1</v>
       </c>
-      <c r="B6" s="115" t="s">
+      <c r="B6" s="112" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="115"/>
-      <c r="D6" s="115"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="115"/>
-      <c r="G6" s="115"/>
+      <c r="C6" s="112"/>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="112"/>
+      <c r="G6" s="112"/>
       <c r="H6" s="66">
         <v>1</v>
       </c>
@@ -4959,19 +4968,19 @@
       <c r="K41" s="64"/>
     </row>
     <row r="42" spans="9:20" x14ac:dyDescent="0.2">
-      <c r="J42" s="114" t="s">
+      <c r="J42" s="116" t="s">
         <v>254</v>
       </c>
-      <c r="K42" s="114"/>
-      <c r="L42" s="114"/>
-      <c r="M42" s="114"/>
-      <c r="N42" s="114"/>
-      <c r="O42" s="114"/>
-      <c r="P42" s="114"/>
-      <c r="Q42" s="114"/>
-      <c r="R42" s="114"/>
-      <c r="S42" s="114"/>
-      <c r="T42" s="114"/>
+      <c r="K42" s="116"/>
+      <c r="L42" s="116"/>
+      <c r="M42" s="116"/>
+      <c r="N42" s="116"/>
+      <c r="O42" s="116"/>
+      <c r="P42" s="116"/>
+      <c r="Q42" s="116"/>
+      <c r="R42" s="116"/>
+      <c r="S42" s="116"/>
+      <c r="T42" s="116"/>
     </row>
     <row r="43" spans="9:20" x14ac:dyDescent="0.2">
       <c r="J43" s="66" t="s">
@@ -5028,11 +5037,11 @@
         <f>IF(L44=L31,2,0)</f>
         <v>2</v>
       </c>
-      <c r="M45" s="111" t="str">
+      <c r="M45" s="113" t="str">
         <f>master!G27</f>
         <v>england</v>
       </c>
-      <c r="Q45" s="111" t="str">
+      <c r="Q45" s="113" t="str">
         <f>master!K27</f>
         <v>france</v>
       </c>
@@ -5053,7 +5062,7 @@
       <c r="L46" s="65" t="s">
         <v>234</v>
       </c>
-      <c r="M46" s="112"/>
+      <c r="M46" s="114"/>
       <c r="O46" s="65" t="s">
         <v>151</v>
       </c>
@@ -5200,11 +5209,11 @@
         <f>IF(L50=L37,2,0)</f>
         <v>0</v>
       </c>
-      <c r="M51" s="111" t="str">
+      <c r="M51" s="113" t="str">
         <f>master!G33</f>
         <v>spain</v>
       </c>
-      <c r="Q51" s="111" t="str">
+      <c r="Q51" s="113" t="str">
         <f>master!K33</f>
         <v>usa</v>
       </c>
@@ -5225,7 +5234,7 @@
       <c r="L52" s="65" t="s">
         <v>236</v>
       </c>
-      <c r="M52" s="112"/>
+      <c r="M52" s="114"/>
       <c r="Q52" s="119"/>
       <c r="R52" s="65" t="s">
         <v>240</v>
@@ -5317,11 +5326,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
     <mergeCell ref="M51:M52"/>
     <mergeCell ref="Q51:Q52"/>
     <mergeCell ref="M32:M33"/>
@@ -5329,6 +5333,11 @@
     <mergeCell ref="J42:T42"/>
     <mergeCell ref="M45:M46"/>
     <mergeCell ref="Q45:Q46"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <conditionalFormatting sqref="H10 N10 H17 N17 H24 N24">
     <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
@@ -5400,15 +5409,15 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="114" t="s">
+      <c r="A2" s="116" t="s">
         <v>228</v>
       </c>
-      <c r="B2" s="114"/>
-      <c r="C2" s="114"/>
-      <c r="D2" s="114"/>
-      <c r="E2" s="114"/>
-      <c r="F2" s="114"/>
-      <c r="G2" s="114"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="122" t="s">
@@ -5584,15 +5593,15 @@
       <c r="G13" s="121"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="114" t="s">
+      <c r="A16" s="116" t="s">
         <v>241</v>
       </c>
-      <c r="B16" s="114"/>
-      <c r="C16" s="114"/>
-      <c r="D16" s="114"/>
-      <c r="E16" s="114"/>
-      <c r="F16" s="114"/>
-      <c r="G16" s="114"/>
+      <c r="B16" s="116"/>
+      <c r="C16" s="116"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="116"/>
+      <c r="G16" s="116"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="120" t="s">
@@ -5769,6 +5778,9 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A20:A21"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="G3:G4"/>
@@ -5784,9 +5796,6 @@
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A20:A21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7065,14 +7074,14 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="68"/>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="112" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
@@ -7083,14 +7092,14 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="77"/>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="112" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
@@ -7101,14 +7110,14 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="72"/>
-      <c r="B4" s="115" t="s">
+      <c r="B4" s="112" t="s">
         <v>143</v>
       </c>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
@@ -7119,14 +7128,14 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="69"/>
-      <c r="B5" s="115" t="s">
+      <c r="B5" s="112" t="s">
         <v>144</v>
       </c>
-      <c r="C5" s="115"/>
-      <c r="D5" s="115"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="115"/>
-      <c r="G5" s="115"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
@@ -7137,14 +7146,14 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="22"/>
-      <c r="B6" s="115" t="s">
+      <c r="B6" s="112" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="115"/>
-      <c r="D6" s="115"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="115"/>
-      <c r="G6" s="115"/>
+      <c r="C6" s="112"/>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="112"/>
+      <c r="G6" s="112"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
@@ -8055,7 +8064,7 @@
       <c r="AE30" s="89"/>
     </row>
     <row r="31" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C31" s="116"/>
+      <c r="C31" s="111"/>
       <c r="D31" s="66" t="s">
         <v>210</v>
       </c>
@@ -8077,7 +8086,7 @@
       </c>
     </row>
     <row r="32" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C32" s="116"/>
+      <c r="C32" s="111"/>
       <c r="D32" s="76" t="s">
         <v>220</v>
       </c>
@@ -8122,7 +8131,7 @@
       <c r="AE33" s="89"/>
     </row>
     <row r="34" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C34" s="116"/>
+      <c r="C34" s="111"/>
       <c r="D34" s="70" t="s">
         <v>211</v>
       </c>
@@ -8149,7 +8158,7 @@
       </c>
     </row>
     <row r="35" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C35" s="116"/>
+      <c r="C35" s="111"/>
       <c r="D35" s="70" t="s">
         <v>216</v>
       </c>
@@ -8196,7 +8205,7 @@
       <c r="AE36" s="89"/>
     </row>
     <row r="37" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C37" s="116"/>
+      <c r="C37" s="111"/>
       <c r="D37" s="66" t="s">
         <v>224</v>
       </c>
@@ -8219,7 +8228,7 @@
       </c>
     </row>
     <row r="38" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C38" s="116"/>
+      <c r="C38" s="111"/>
       <c r="D38" s="76" t="s">
         <v>255</v>
       </c>
@@ -8244,7 +8253,7 @@
       <c r="X38" s="76" t="s">
         <v>226</v>
       </c>
-      <c r="AE38" s="116"/>
+      <c r="AE38" s="111"/>
     </row>
     <row r="39" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C39"/>
@@ -8258,10 +8267,10 @@
       </c>
       <c r="W39" s="66"/>
       <c r="X39" s="66"/>
-      <c r="AE39" s="116"/>
+      <c r="AE39" s="111"/>
     </row>
     <row r="40" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C40" s="116"/>
+      <c r="C40" s="111"/>
       <c r="D40" s="70" t="s">
         <v>219</v>
       </c>
@@ -8284,7 +8293,7 @@
       </c>
     </row>
     <row r="41" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C41" s="116"/>
+      <c r="C41" s="111"/>
       <c r="D41" s="70" t="s">
         <v>222</v>
       </c>
@@ -8305,29 +8314,29 @@
       </c>
     </row>
     <row r="43" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="D43" s="114" t="s">
+      <c r="D43" s="116" t="s">
         <v>254</v>
       </c>
-      <c r="E43" s="114"/>
-      <c r="F43" s="114"/>
-      <c r="G43" s="114"/>
-      <c r="H43" s="114"/>
-      <c r="I43" s="114"/>
-      <c r="J43" s="114"/>
-      <c r="K43" s="114"/>
-      <c r="L43" s="114"/>
-      <c r="M43" s="114"/>
-      <c r="N43" s="114"/>
-      <c r="O43" s="114"/>
-      <c r="P43" s="114"/>
-      <c r="Q43" s="114"/>
-      <c r="R43" s="114"/>
-      <c r="S43" s="114"/>
-      <c r="T43" s="114"/>
-      <c r="U43" s="114"/>
-      <c r="V43" s="114"/>
-      <c r="W43" s="114"/>
-      <c r="X43" s="114"/>
+      <c r="E43" s="116"/>
+      <c r="F43" s="116"/>
+      <c r="G43" s="116"/>
+      <c r="H43" s="116"/>
+      <c r="I43" s="116"/>
+      <c r="J43" s="116"/>
+      <c r="K43" s="116"/>
+      <c r="L43" s="116"/>
+      <c r="M43" s="116"/>
+      <c r="N43" s="116"/>
+      <c r="O43" s="116"/>
+      <c r="P43" s="116"/>
+      <c r="Q43" s="116"/>
+      <c r="R43" s="116"/>
+      <c r="S43" s="116"/>
+      <c r="T43" s="116"/>
+      <c r="U43" s="116"/>
+      <c r="V43" s="116"/>
+      <c r="W43" s="116"/>
+      <c r="X43" s="116"/>
     </row>
     <row r="44" spans="3:31" x14ac:dyDescent="0.2">
       <c r="D44" s="66" t="s">
@@ -8386,12 +8395,12 @@
         <f>IF(F45=F32,2,0)</f>
         <v>2</v>
       </c>
-      <c r="G46" s="111" t="str">
+      <c r="G46" s="113" t="str">
         <f>master!G27</f>
         <v>england</v>
       </c>
       <c r="M46" s="64"/>
-      <c r="P46" s="113" t="str">
+      <c r="P46" s="115" t="str">
         <f>master!K27</f>
         <v>france</v>
       </c>
@@ -8412,12 +8421,12 @@
       <c r="F47" s="65" t="s">
         <v>234</v>
       </c>
-      <c r="G47" s="112"/>
+      <c r="G47" s="114"/>
       <c r="M47" s="67"/>
       <c r="N47" s="65" t="s">
         <v>151</v>
       </c>
-      <c r="P47" s="113"/>
+      <c r="P47" s="115"/>
       <c r="V47" s="90" t="s">
         <v>238</v>
       </c>
@@ -8446,7 +8455,7 @@
       <c r="L48" s="65" t="s">
         <v>224</v>
       </c>
-      <c r="N48" s="113" t="str">
+      <c r="N48" s="115" t="str">
         <f>master!I29</f>
         <v>france</v>
       </c>
@@ -8475,12 +8484,12 @@
         <f>IF(F48=F35,2,0)</f>
         <v>2</v>
       </c>
-      <c r="L49" s="113" t="str">
+      <c r="L49" s="115" t="str">
         <f>master!H30</f>
         <v>england</v>
       </c>
-      <c r="N49" s="113"/>
-      <c r="O49" s="113" t="str">
+      <c r="N49" s="115"/>
+      <c r="O49" s="115" t="str">
         <f>master!J30</f>
         <v>france</v>
       </c>
@@ -8501,12 +8510,12 @@
       <c r="F50" s="65" t="s">
         <v>235</v>
       </c>
-      <c r="L50" s="113"/>
+      <c r="L50" s="115"/>
       <c r="N50" s="64">
         <f>IF(N48=N35,10,0)</f>
         <v>10</v>
       </c>
-      <c r="O50" s="113"/>
+      <c r="O50" s="115"/>
       <c r="V50" s="65" t="s">
         <v>239</v>
       </c>
@@ -8559,11 +8568,11 @@
         <f>IF(F51=F38,2,0)</f>
         <v>2</v>
       </c>
-      <c r="G52" s="111" t="str">
+      <c r="G52" s="113" t="str">
         <f>master!G33</f>
         <v>spain</v>
       </c>
-      <c r="P52" s="113" t="str">
+      <c r="P52" s="115" t="str">
         <f>master!K33</f>
         <v>usa</v>
       </c>
@@ -8584,8 +8593,8 @@
       <c r="F53" s="65" t="s">
         <v>236</v>
       </c>
-      <c r="G53" s="112"/>
-      <c r="P53" s="113"/>
+      <c r="G53" s="114"/>
+      <c r="P53" s="115"/>
       <c r="V53" s="65" t="s">
         <v>240</v>
       </c>
@@ -8705,6 +8714,19 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="P52:P53"/>
+    <mergeCell ref="D43:X43"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="P46:P47"/>
+    <mergeCell ref="N48:N49"/>
+    <mergeCell ref="L49:L50"/>
+    <mergeCell ref="O49:O50"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="AE38:AE39"/>
     <mergeCell ref="G39:G40"/>
@@ -8717,19 +8739,6 @@
     <mergeCell ref="L36:L37"/>
     <mergeCell ref="O36:O37"/>
     <mergeCell ref="N35:N36"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="P52:P53"/>
-    <mergeCell ref="D43:X43"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="P46:P47"/>
-    <mergeCell ref="N48:N49"/>
-    <mergeCell ref="L49:L50"/>
-    <mergeCell ref="O49:O50"/>
   </mergeCells>
   <conditionalFormatting sqref="L10 V10 L17 V17 L24 V24">
     <cfRule type="cellIs" dxfId="32" priority="6" operator="equal">
@@ -8791,14 +8800,14 @@
       <c r="A2" s="70">
         <v>5</v>
       </c>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="112" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
       <c r="H2" s="66">
         <v>5</v>
       </c>
@@ -8807,14 +8816,14 @@
       <c r="A3" s="78">
         <v>4</v>
       </c>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="112" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
       <c r="H3" s="66">
         <v>4</v>
       </c>
@@ -8823,14 +8832,14 @@
       <c r="A4" s="73">
         <v>3</v>
       </c>
-      <c r="B4" s="115" t="s">
+      <c r="B4" s="112" t="s">
         <v>143</v>
       </c>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
       <c r="H4" s="66">
         <v>3</v>
       </c>
@@ -8839,14 +8848,14 @@
       <c r="A5" s="79">
         <v>2</v>
       </c>
-      <c r="B5" s="115" t="s">
+      <c r="B5" s="112" t="s">
         <v>144</v>
       </c>
-      <c r="C5" s="115"/>
-      <c r="D5" s="115"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="115"/>
-      <c r="G5" s="115"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
       <c r="H5" s="66">
         <v>2</v>
       </c>
@@ -8855,14 +8864,14 @@
       <c r="A6" s="71">
         <v>1</v>
       </c>
-      <c r="B6" s="115" t="s">
+      <c r="B6" s="112" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="115"/>
-      <c r="D6" s="115"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="115"/>
-      <c r="G6" s="115"/>
+      <c r="C6" s="112"/>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="112"/>
+      <c r="G6" s="112"/>
       <c r="H6" s="66">
         <v>1</v>
       </c>
@@ -9702,19 +9711,19 @@
       <c r="K41" s="64"/>
     </row>
     <row r="42" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="J42" s="114" t="s">
+      <c r="J42" s="116" t="s">
         <v>254</v>
       </c>
-      <c r="K42" s="114"/>
-      <c r="L42" s="114"/>
-      <c r="M42" s="114"/>
-      <c r="N42" s="114"/>
-      <c r="O42" s="114"/>
-      <c r="P42" s="114"/>
-      <c r="Q42" s="114"/>
-      <c r="R42" s="114"/>
-      <c r="S42" s="114"/>
-      <c r="T42" s="114"/>
+      <c r="K42" s="116"/>
+      <c r="L42" s="116"/>
+      <c r="M42" s="116"/>
+      <c r="N42" s="116"/>
+      <c r="O42" s="116"/>
+      <c r="P42" s="116"/>
+      <c r="Q42" s="116"/>
+      <c r="R42" s="116"/>
+      <c r="S42" s="116"/>
+      <c r="T42" s="116"/>
       <c r="U42" s="80"/>
       <c r="V42" s="80"/>
       <c r="W42" s="80"/>
@@ -9781,11 +9790,11 @@
         <f>IF(L44=L31,2,0)</f>
         <v>0</v>
       </c>
-      <c r="M45" s="111" t="str">
+      <c r="M45" s="113" t="str">
         <f>master!G27</f>
         <v>england</v>
       </c>
-      <c r="Q45" s="111" t="str">
+      <c r="Q45" s="113" t="str">
         <f>master!K27</f>
         <v>france</v>
       </c>
@@ -9806,7 +9815,7 @@
       <c r="L46" s="65" t="s">
         <v>234</v>
       </c>
-      <c r="M46" s="112"/>
+      <c r="M46" s="114"/>
       <c r="O46" s="65" t="s">
         <v>151</v>
       </c>
@@ -9953,11 +9962,11 @@
         <f>IF(L50=L37,2,0)</f>
         <v>2</v>
       </c>
-      <c r="M51" s="111" t="str">
+      <c r="M51" s="113" t="str">
         <f>master!G33</f>
         <v>spain</v>
       </c>
-      <c r="Q51" s="111" t="str">
+      <c r="Q51" s="113" t="str">
         <f>master!K33</f>
         <v>usa</v>
       </c>
@@ -9978,7 +9987,7 @@
       <c r="L52" s="65" t="s">
         <v>236</v>
       </c>
-      <c r="M52" s="112"/>
+      <c r="M52" s="114"/>
       <c r="Q52" s="119"/>
       <c r="R52" s="65" t="s">
         <v>240</v>
@@ -10072,6 +10081,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="M51:M52"/>
+    <mergeCell ref="J42:T42"/>
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="M45:M46"/>
+    <mergeCell ref="Q51:Q52"/>
     <mergeCell ref="M32:M33"/>
     <mergeCell ref="Q45:Q46"/>
     <mergeCell ref="B2:G2"/>
@@ -10079,11 +10093,6 @@
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B5:G5"/>
     <mergeCell ref="B6:G6"/>
-    <mergeCell ref="M51:M52"/>
-    <mergeCell ref="J42:T42"/>
-    <mergeCell ref="M38:M39"/>
-    <mergeCell ref="M45:M46"/>
-    <mergeCell ref="Q51:Q52"/>
   </mergeCells>
   <conditionalFormatting sqref="H10 M10 H17 M17 H24 M24">
     <cfRule type="cellIs" dxfId="27" priority="14" operator="equal">
@@ -10166,14 +10175,14 @@
       <c r="A2" s="70">
         <v>5</v>
       </c>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="112" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
       <c r="H2" s="66">
         <v>5</v>
       </c>
@@ -10182,14 +10191,14 @@
       <c r="A3" s="78">
         <v>4</v>
       </c>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="112" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
       <c r="H3" s="66">
         <v>4</v>
       </c>
@@ -10198,14 +10207,14 @@
       <c r="A4" s="73">
         <v>3</v>
       </c>
-      <c r="B4" s="115" t="s">
+      <c r="B4" s="112" t="s">
         <v>143</v>
       </c>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
       <c r="H4" s="66">
         <v>3</v>
       </c>
@@ -10214,14 +10223,14 @@
       <c r="A5" s="79">
         <v>2</v>
       </c>
-      <c r="B5" s="115" t="s">
+      <c r="B5" s="112" t="s">
         <v>144</v>
       </c>
-      <c r="C5" s="115"/>
-      <c r="D5" s="115"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="115"/>
-      <c r="G5" s="115"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
       <c r="H5" s="66">
         <v>2</v>
       </c>
@@ -10230,14 +10239,14 @@
       <c r="A6" s="71">
         <v>1</v>
       </c>
-      <c r="B6" s="115" t="s">
+      <c r="B6" s="112" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="115"/>
-      <c r="D6" s="115"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="115"/>
-      <c r="G6" s="115"/>
+      <c r="C6" s="112"/>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="112"/>
+      <c r="G6" s="112"/>
       <c r="H6" s="66">
         <v>1</v>
       </c>
@@ -11057,19 +11066,19 @@
       <c r="K41" s="64"/>
     </row>
     <row r="42" spans="9:20" x14ac:dyDescent="0.2">
-      <c r="J42" s="114" t="s">
+      <c r="J42" s="116" t="s">
         <v>254</v>
       </c>
-      <c r="K42" s="114"/>
-      <c r="L42" s="114"/>
-      <c r="M42" s="114"/>
-      <c r="N42" s="114"/>
-      <c r="O42" s="114"/>
-      <c r="P42" s="114"/>
-      <c r="Q42" s="114"/>
-      <c r="R42" s="114"/>
-      <c r="S42" s="114"/>
-      <c r="T42" s="114"/>
+      <c r="K42" s="116"/>
+      <c r="L42" s="116"/>
+      <c r="M42" s="116"/>
+      <c r="N42" s="116"/>
+      <c r="O42" s="116"/>
+      <c r="P42" s="116"/>
+      <c r="Q42" s="116"/>
+      <c r="R42" s="116"/>
+      <c r="S42" s="116"/>
+      <c r="T42" s="116"/>
     </row>
     <row r="43" spans="9:20" x14ac:dyDescent="0.2">
       <c r="J43" s="66" t="s">
@@ -11126,11 +11135,11 @@
         <f>IF(L44=L31,2,0)</f>
         <v>2</v>
       </c>
-      <c r="M45" s="111" t="str">
+      <c r="M45" s="113" t="str">
         <f>master!G27</f>
         <v>england</v>
       </c>
-      <c r="Q45" s="111" t="str">
+      <c r="Q45" s="113" t="str">
         <f>master!K27</f>
         <v>france</v>
       </c>
@@ -11151,7 +11160,7 @@
       <c r="L46" s="65" t="s">
         <v>234</v>
       </c>
-      <c r="M46" s="112"/>
+      <c r="M46" s="114"/>
       <c r="O46" s="65" t="s">
         <v>151</v>
       </c>
@@ -11298,11 +11307,11 @@
         <f>IF(L50=L37,2,0)</f>
         <v>0</v>
       </c>
-      <c r="M51" s="111" t="str">
+      <c r="M51" s="113" t="str">
         <f>master!G33</f>
         <v>spain</v>
       </c>
-      <c r="Q51" s="111" t="str">
+      <c r="Q51" s="113" t="str">
         <f>master!K33</f>
         <v>usa</v>
       </c>
@@ -11323,7 +11332,7 @@
       <c r="L52" s="65" t="s">
         <v>236</v>
       </c>
-      <c r="M52" s="112"/>
+      <c r="M52" s="114"/>
       <c r="Q52" s="119"/>
       <c r="R52" s="65" t="s">
         <v>240</v>
@@ -11415,11 +11424,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
     <mergeCell ref="M51:M52"/>
     <mergeCell ref="Q51:Q52"/>
     <mergeCell ref="M32:M33"/>
@@ -11427,6 +11431,11 @@
     <mergeCell ref="J42:T42"/>
     <mergeCell ref="M45:M46"/>
     <mergeCell ref="Q45:Q46"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <conditionalFormatting sqref="H10 N10 H17 N17 H24 N24">
     <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">

</xml_diff>

<commit_message>
route work complete for header/navBar
</commit_message>
<xml_diff>
--- a/excel-docs/euro - lifecycle info.xlsx
+++ b/excel-docs/euro - lifecycle info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joseph.collins/Documents/personal-projects/euro/2024_euro/excel-docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839C5568-011B-C342-A416-A7937D7349C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2E044C-E03C-0C4F-AD39-C24FCBCF3DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34560" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D89656BD-B983-D041-A997-C1184058734E}"/>
   </bookViews>
@@ -1510,6 +1510,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1521,10 +1525,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2102,7 +2102,7 @@
   </sheetPr>
   <dimension ref="A1:F107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="160" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2734,14 +2734,14 @@
       <c r="A2" s="70">
         <v>5</v>
       </c>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="112" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
       <c r="H2" s="66">
         <v>5</v>
       </c>
@@ -2750,14 +2750,14 @@
       <c r="A3" s="78">
         <v>4</v>
       </c>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="112" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
       <c r="H3" s="66">
         <v>4</v>
       </c>
@@ -2766,14 +2766,14 @@
       <c r="A4" s="73">
         <v>3</v>
       </c>
-      <c r="B4" s="115" t="s">
+      <c r="B4" s="112" t="s">
         <v>143</v>
       </c>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
       <c r="H4" s="66">
         <v>3</v>
       </c>
@@ -2782,14 +2782,14 @@
       <c r="A5" s="79">
         <v>2</v>
       </c>
-      <c r="B5" s="115" t="s">
+      <c r="B5" s="112" t="s">
         <v>144</v>
       </c>
-      <c r="C5" s="115"/>
-      <c r="D5" s="115"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="115"/>
-      <c r="G5" s="115"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
       <c r="H5" s="66">
         <v>2</v>
       </c>
@@ -2798,14 +2798,14 @@
       <c r="A6" s="71">
         <v>1</v>
       </c>
-      <c r="B6" s="115" t="s">
+      <c r="B6" s="112" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="115"/>
-      <c r="D6" s="115"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="115"/>
-      <c r="G6" s="115"/>
+      <c r="C6" s="112"/>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="112"/>
+      <c r="G6" s="112"/>
       <c r="H6" s="66">
         <v>1</v>
       </c>
@@ -3625,19 +3625,19 @@
       <c r="K41" s="64"/>
     </row>
     <row r="42" spans="9:20" x14ac:dyDescent="0.2">
-      <c r="J42" s="114" t="s">
+      <c r="J42" s="116" t="s">
         <v>254</v>
       </c>
-      <c r="K42" s="114"/>
-      <c r="L42" s="114"/>
-      <c r="M42" s="114"/>
-      <c r="N42" s="114"/>
-      <c r="O42" s="114"/>
-      <c r="P42" s="114"/>
-      <c r="Q42" s="114"/>
-      <c r="R42" s="114"/>
-      <c r="S42" s="114"/>
-      <c r="T42" s="114"/>
+      <c r="K42" s="116"/>
+      <c r="L42" s="116"/>
+      <c r="M42" s="116"/>
+      <c r="N42" s="116"/>
+      <c r="O42" s="116"/>
+      <c r="P42" s="116"/>
+      <c r="Q42" s="116"/>
+      <c r="R42" s="116"/>
+      <c r="S42" s="116"/>
+      <c r="T42" s="116"/>
     </row>
     <row r="43" spans="9:20" x14ac:dyDescent="0.2">
       <c r="J43" s="66" t="s">
@@ -3694,11 +3694,11 @@
         <f>IF(L44=L31,2,0)</f>
         <v>0</v>
       </c>
-      <c r="M45" s="111" t="str">
+      <c r="M45" s="113" t="str">
         <f>master!G27</f>
         <v>england</v>
       </c>
-      <c r="Q45" s="111" t="str">
+      <c r="Q45" s="113" t="str">
         <f>master!K27</f>
         <v>france</v>
       </c>
@@ -3719,7 +3719,7 @@
       <c r="L46" s="65" t="s">
         <v>234</v>
       </c>
-      <c r="M46" s="112"/>
+      <c r="M46" s="114"/>
       <c r="O46" s="65" t="s">
         <v>151</v>
       </c>
@@ -3866,11 +3866,11 @@
         <f>IF(L50=L37,2,0)</f>
         <v>2</v>
       </c>
-      <c r="M51" s="111" t="str">
+      <c r="M51" s="113" t="str">
         <f>master!G33</f>
         <v>spain</v>
       </c>
-      <c r="Q51" s="111" t="str">
+      <c r="Q51" s="113" t="str">
         <f>master!K33</f>
         <v>usa</v>
       </c>
@@ -3891,7 +3891,7 @@
       <c r="L52" s="65" t="s">
         <v>236</v>
       </c>
-      <c r="M52" s="112"/>
+      <c r="M52" s="114"/>
       <c r="Q52" s="119"/>
       <c r="R52" s="65" t="s">
         <v>240</v>
@@ -3983,11 +3983,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
     <mergeCell ref="M51:M52"/>
     <mergeCell ref="Q51:Q52"/>
     <mergeCell ref="M32:M33"/>
@@ -3995,6 +3990,11 @@
     <mergeCell ref="J42:T42"/>
     <mergeCell ref="M45:M46"/>
     <mergeCell ref="Q45:Q46"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <conditionalFormatting sqref="H10 N10 H17 N17 H24 N24">
     <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
@@ -4077,14 +4077,14 @@
       <c r="A2" s="70">
         <v>5</v>
       </c>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="112" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
       <c r="H2" s="66">
         <v>5</v>
       </c>
@@ -4093,14 +4093,14 @@
       <c r="A3" s="78">
         <v>4</v>
       </c>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="112" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
       <c r="H3" s="66">
         <v>4</v>
       </c>
@@ -4109,14 +4109,14 @@
       <c r="A4" s="73">
         <v>3</v>
       </c>
-      <c r="B4" s="115" t="s">
+      <c r="B4" s="112" t="s">
         <v>143</v>
       </c>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
       <c r="H4" s="66">
         <v>3</v>
       </c>
@@ -4125,14 +4125,14 @@
       <c r="A5" s="79">
         <v>2</v>
       </c>
-      <c r="B5" s="115" t="s">
+      <c r="B5" s="112" t="s">
         <v>144</v>
       </c>
-      <c r="C5" s="115"/>
-      <c r="D5" s="115"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="115"/>
-      <c r="G5" s="115"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
       <c r="H5" s="66">
         <v>2</v>
       </c>
@@ -4141,14 +4141,14 @@
       <c r="A6" s="71">
         <v>1</v>
       </c>
-      <c r="B6" s="115" t="s">
+      <c r="B6" s="112" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="115"/>
-      <c r="D6" s="115"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="115"/>
-      <c r="G6" s="115"/>
+      <c r="C6" s="112"/>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="112"/>
+      <c r="G6" s="112"/>
       <c r="H6" s="66">
         <v>1</v>
       </c>
@@ -4968,19 +4968,19 @@
       <c r="K41" s="64"/>
     </row>
     <row r="42" spans="9:20" x14ac:dyDescent="0.2">
-      <c r="J42" s="114" t="s">
+      <c r="J42" s="116" t="s">
         <v>254</v>
       </c>
-      <c r="K42" s="114"/>
-      <c r="L42" s="114"/>
-      <c r="M42" s="114"/>
-      <c r="N42" s="114"/>
-      <c r="O42" s="114"/>
-      <c r="P42" s="114"/>
-      <c r="Q42" s="114"/>
-      <c r="R42" s="114"/>
-      <c r="S42" s="114"/>
-      <c r="T42" s="114"/>
+      <c r="K42" s="116"/>
+      <c r="L42" s="116"/>
+      <c r="M42" s="116"/>
+      <c r="N42" s="116"/>
+      <c r="O42" s="116"/>
+      <c r="P42" s="116"/>
+      <c r="Q42" s="116"/>
+      <c r="R42" s="116"/>
+      <c r="S42" s="116"/>
+      <c r="T42" s="116"/>
     </row>
     <row r="43" spans="9:20" x14ac:dyDescent="0.2">
       <c r="J43" s="66" t="s">
@@ -5037,11 +5037,11 @@
         <f>IF(L44=L31,2,0)</f>
         <v>2</v>
       </c>
-      <c r="M45" s="111" t="str">
+      <c r="M45" s="113" t="str">
         <f>master!G27</f>
         <v>england</v>
       </c>
-      <c r="Q45" s="111" t="str">
+      <c r="Q45" s="113" t="str">
         <f>master!K27</f>
         <v>france</v>
       </c>
@@ -5062,7 +5062,7 @@
       <c r="L46" s="65" t="s">
         <v>234</v>
       </c>
-      <c r="M46" s="112"/>
+      <c r="M46" s="114"/>
       <c r="O46" s="65" t="s">
         <v>151</v>
       </c>
@@ -5209,11 +5209,11 @@
         <f>IF(L50=L37,2,0)</f>
         <v>0</v>
       </c>
-      <c r="M51" s="111" t="str">
+      <c r="M51" s="113" t="str">
         <f>master!G33</f>
         <v>spain</v>
       </c>
-      <c r="Q51" s="111" t="str">
+      <c r="Q51" s="113" t="str">
         <f>master!K33</f>
         <v>usa</v>
       </c>
@@ -5234,7 +5234,7 @@
       <c r="L52" s="65" t="s">
         <v>236</v>
       </c>
-      <c r="M52" s="112"/>
+      <c r="M52" s="114"/>
       <c r="Q52" s="119"/>
       <c r="R52" s="65" t="s">
         <v>240</v>
@@ -5326,11 +5326,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
     <mergeCell ref="M51:M52"/>
     <mergeCell ref="Q51:Q52"/>
     <mergeCell ref="M32:M33"/>
@@ -5338,6 +5333,11 @@
     <mergeCell ref="J42:T42"/>
     <mergeCell ref="M45:M46"/>
     <mergeCell ref="Q45:Q46"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <conditionalFormatting sqref="H10 N10 H17 N17 H24 N24">
     <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
@@ -5409,15 +5409,15 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="114" t="s">
+      <c r="A2" s="116" t="s">
         <v>228</v>
       </c>
-      <c r="B2" s="114"/>
-      <c r="C2" s="114"/>
-      <c r="D2" s="114"/>
-      <c r="E2" s="114"/>
-      <c r="F2" s="114"/>
-      <c r="G2" s="114"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="122" t="s">
@@ -5593,15 +5593,15 @@
       <c r="G13" s="121"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="114" t="s">
+      <c r="A16" s="116" t="s">
         <v>241</v>
       </c>
-      <c r="B16" s="114"/>
-      <c r="C16" s="114"/>
-      <c r="D16" s="114"/>
-      <c r="E16" s="114"/>
-      <c r="F16" s="114"/>
-      <c r="G16" s="114"/>
+      <c r="B16" s="116"/>
+      <c r="C16" s="116"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="116"/>
+      <c r="G16" s="116"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="120" t="s">
@@ -5778,11 +5778,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A20:A21"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="G3:G4"/>
@@ -5796,6 +5791,11 @@
     <mergeCell ref="A16:G16"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A20:A21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7074,14 +7074,14 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="68"/>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="112" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
@@ -7092,14 +7092,14 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="77"/>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="112" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
@@ -7110,14 +7110,14 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="72"/>
-      <c r="B4" s="115" t="s">
+      <c r="B4" s="112" t="s">
         <v>143</v>
       </c>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
@@ -7128,14 +7128,14 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="69"/>
-      <c r="B5" s="115" t="s">
+      <c r="B5" s="112" t="s">
         <v>144</v>
       </c>
-      <c r="C5" s="115"/>
-      <c r="D5" s="115"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="115"/>
-      <c r="G5" s="115"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
@@ -7146,14 +7146,14 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="22"/>
-      <c r="B6" s="115" t="s">
+      <c r="B6" s="112" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="115"/>
-      <c r="D6" s="115"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="115"/>
-      <c r="G6" s="115"/>
+      <c r="C6" s="112"/>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="112"/>
+      <c r="G6" s="112"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
@@ -8064,7 +8064,7 @@
       <c r="AE30" s="89"/>
     </row>
     <row r="31" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C31" s="116"/>
+      <c r="C31" s="111"/>
       <c r="D31" s="66" t="s">
         <v>210</v>
       </c>
@@ -8086,7 +8086,7 @@
       </c>
     </row>
     <row r="32" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C32" s="116"/>
+      <c r="C32" s="111"/>
       <c r="D32" s="76" t="s">
         <v>220</v>
       </c>
@@ -8131,7 +8131,7 @@
       <c r="AE33" s="89"/>
     </row>
     <row r="34" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C34" s="116"/>
+      <c r="C34" s="111"/>
       <c r="D34" s="70" t="s">
         <v>211</v>
       </c>
@@ -8158,7 +8158,7 @@
       </c>
     </row>
     <row r="35" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C35" s="116"/>
+      <c r="C35" s="111"/>
       <c r="D35" s="70" t="s">
         <v>216</v>
       </c>
@@ -8205,7 +8205,7 @@
       <c r="AE36" s="89"/>
     </row>
     <row r="37" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C37" s="116"/>
+      <c r="C37" s="111"/>
       <c r="D37" s="66" t="s">
         <v>224</v>
       </c>
@@ -8228,7 +8228,7 @@
       </c>
     </row>
     <row r="38" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C38" s="116"/>
+      <c r="C38" s="111"/>
       <c r="D38" s="76" t="s">
         <v>255</v>
       </c>
@@ -8253,7 +8253,7 @@
       <c r="X38" s="76" t="s">
         <v>226</v>
       </c>
-      <c r="AE38" s="116"/>
+      <c r="AE38" s="111"/>
     </row>
     <row r="39" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C39"/>
@@ -8267,10 +8267,10 @@
       </c>
       <c r="W39" s="66"/>
       <c r="X39" s="66"/>
-      <c r="AE39" s="116"/>
+      <c r="AE39" s="111"/>
     </row>
     <row r="40" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C40" s="116"/>
+      <c r="C40" s="111"/>
       <c r="D40" s="70" t="s">
         <v>219</v>
       </c>
@@ -8293,7 +8293,7 @@
       </c>
     </row>
     <row r="41" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C41" s="116"/>
+      <c r="C41" s="111"/>
       <c r="D41" s="70" t="s">
         <v>222</v>
       </c>
@@ -8314,29 +8314,29 @@
       </c>
     </row>
     <row r="43" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="D43" s="114" t="s">
+      <c r="D43" s="116" t="s">
         <v>254</v>
       </c>
-      <c r="E43" s="114"/>
-      <c r="F43" s="114"/>
-      <c r="G43" s="114"/>
-      <c r="H43" s="114"/>
-      <c r="I43" s="114"/>
-      <c r="J43" s="114"/>
-      <c r="K43" s="114"/>
-      <c r="L43" s="114"/>
-      <c r="M43" s="114"/>
-      <c r="N43" s="114"/>
-      <c r="O43" s="114"/>
-      <c r="P43" s="114"/>
-      <c r="Q43" s="114"/>
-      <c r="R43" s="114"/>
-      <c r="S43" s="114"/>
-      <c r="T43" s="114"/>
-      <c r="U43" s="114"/>
-      <c r="V43" s="114"/>
-      <c r="W43" s="114"/>
-      <c r="X43" s="114"/>
+      <c r="E43" s="116"/>
+      <c r="F43" s="116"/>
+      <c r="G43" s="116"/>
+      <c r="H43" s="116"/>
+      <c r="I43" s="116"/>
+      <c r="J43" s="116"/>
+      <c r="K43" s="116"/>
+      <c r="L43" s="116"/>
+      <c r="M43" s="116"/>
+      <c r="N43" s="116"/>
+      <c r="O43" s="116"/>
+      <c r="P43" s="116"/>
+      <c r="Q43" s="116"/>
+      <c r="R43" s="116"/>
+      <c r="S43" s="116"/>
+      <c r="T43" s="116"/>
+      <c r="U43" s="116"/>
+      <c r="V43" s="116"/>
+      <c r="W43" s="116"/>
+      <c r="X43" s="116"/>
     </row>
     <row r="44" spans="3:31" x14ac:dyDescent="0.2">
       <c r="D44" s="66" t="s">
@@ -8395,12 +8395,12 @@
         <f>IF(F45=F32,2,0)</f>
         <v>2</v>
       </c>
-      <c r="G46" s="111" t="str">
+      <c r="G46" s="113" t="str">
         <f>master!G27</f>
         <v>england</v>
       </c>
       <c r="M46" s="64"/>
-      <c r="P46" s="113" t="str">
+      <c r="P46" s="115" t="str">
         <f>master!K27</f>
         <v>france</v>
       </c>
@@ -8421,12 +8421,12 @@
       <c r="F47" s="65" t="s">
         <v>234</v>
       </c>
-      <c r="G47" s="112"/>
+      <c r="G47" s="114"/>
       <c r="M47" s="67"/>
       <c r="N47" s="65" t="s">
         <v>151</v>
       </c>
-      <c r="P47" s="113"/>
+      <c r="P47" s="115"/>
       <c r="V47" s="90" t="s">
         <v>238</v>
       </c>
@@ -8455,7 +8455,7 @@
       <c r="L48" s="65" t="s">
         <v>224</v>
       </c>
-      <c r="N48" s="113" t="str">
+      <c r="N48" s="115" t="str">
         <f>master!I29</f>
         <v>france</v>
       </c>
@@ -8484,12 +8484,12 @@
         <f>IF(F48=F35,2,0)</f>
         <v>2</v>
       </c>
-      <c r="L49" s="113" t="str">
+      <c r="L49" s="115" t="str">
         <f>master!H30</f>
         <v>england</v>
       </c>
-      <c r="N49" s="113"/>
-      <c r="O49" s="113" t="str">
+      <c r="N49" s="115"/>
+      <c r="O49" s="115" t="str">
         <f>master!J30</f>
         <v>france</v>
       </c>
@@ -8510,12 +8510,12 @@
       <c r="F50" s="65" t="s">
         <v>235</v>
       </c>
-      <c r="L50" s="113"/>
+      <c r="L50" s="115"/>
       <c r="N50" s="64">
         <f>IF(N48=N35,10,0)</f>
         <v>10</v>
       </c>
-      <c r="O50" s="113"/>
+      <c r="O50" s="115"/>
       <c r="V50" s="65" t="s">
         <v>239</v>
       </c>
@@ -8568,11 +8568,11 @@
         <f>IF(F51=F38,2,0)</f>
         <v>2</v>
       </c>
-      <c r="G52" s="111" t="str">
+      <c r="G52" s="113" t="str">
         <f>master!G33</f>
         <v>spain</v>
       </c>
-      <c r="P52" s="113" t="str">
+      <c r="P52" s="115" t="str">
         <f>master!K33</f>
         <v>usa</v>
       </c>
@@ -8593,8 +8593,8 @@
       <c r="F53" s="65" t="s">
         <v>236</v>
       </c>
-      <c r="G53" s="112"/>
-      <c r="P53" s="113"/>
+      <c r="G53" s="114"/>
+      <c r="P53" s="115"/>
       <c r="V53" s="65" t="s">
         <v>240</v>
       </c>
@@ -8714,6 +8714,19 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="P52:P53"/>
+    <mergeCell ref="D43:X43"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="P46:P47"/>
+    <mergeCell ref="N48:N49"/>
+    <mergeCell ref="L49:L50"/>
+    <mergeCell ref="O49:O50"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="AE38:AE39"/>
     <mergeCell ref="G39:G40"/>
@@ -8726,19 +8739,6 @@
     <mergeCell ref="L36:L37"/>
     <mergeCell ref="O36:O37"/>
     <mergeCell ref="N35:N36"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="P52:P53"/>
-    <mergeCell ref="D43:X43"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="P46:P47"/>
-    <mergeCell ref="N48:N49"/>
-    <mergeCell ref="L49:L50"/>
-    <mergeCell ref="O49:O50"/>
   </mergeCells>
   <conditionalFormatting sqref="L10 V10 L17 V17 L24 V24">
     <cfRule type="cellIs" dxfId="32" priority="6" operator="equal">
@@ -8800,14 +8800,14 @@
       <c r="A2" s="70">
         <v>5</v>
       </c>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="112" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
       <c r="H2" s="66">
         <v>5</v>
       </c>
@@ -8816,14 +8816,14 @@
       <c r="A3" s="78">
         <v>4</v>
       </c>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="112" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
       <c r="H3" s="66">
         <v>4</v>
       </c>
@@ -8832,14 +8832,14 @@
       <c r="A4" s="73">
         <v>3</v>
       </c>
-      <c r="B4" s="115" t="s">
+      <c r="B4" s="112" t="s">
         <v>143</v>
       </c>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
       <c r="H4" s="66">
         <v>3</v>
       </c>
@@ -8848,14 +8848,14 @@
       <c r="A5" s="79">
         <v>2</v>
       </c>
-      <c r="B5" s="115" t="s">
+      <c r="B5" s="112" t="s">
         <v>144</v>
       </c>
-      <c r="C5" s="115"/>
-      <c r="D5" s="115"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="115"/>
-      <c r="G5" s="115"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
       <c r="H5" s="66">
         <v>2</v>
       </c>
@@ -8864,14 +8864,14 @@
       <c r="A6" s="71">
         <v>1</v>
       </c>
-      <c r="B6" s="115" t="s">
+      <c r="B6" s="112" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="115"/>
-      <c r="D6" s="115"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="115"/>
-      <c r="G6" s="115"/>
+      <c r="C6" s="112"/>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="112"/>
+      <c r="G6" s="112"/>
       <c r="H6" s="66">
         <v>1</v>
       </c>
@@ -9711,19 +9711,19 @@
       <c r="K41" s="64"/>
     </row>
     <row r="42" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="J42" s="114" t="s">
+      <c r="J42" s="116" t="s">
         <v>254</v>
       </c>
-      <c r="K42" s="114"/>
-      <c r="L42" s="114"/>
-      <c r="M42" s="114"/>
-      <c r="N42" s="114"/>
-      <c r="O42" s="114"/>
-      <c r="P42" s="114"/>
-      <c r="Q42" s="114"/>
-      <c r="R42" s="114"/>
-      <c r="S42" s="114"/>
-      <c r="T42" s="114"/>
+      <c r="K42" s="116"/>
+      <c r="L42" s="116"/>
+      <c r="M42" s="116"/>
+      <c r="N42" s="116"/>
+      <c r="O42" s="116"/>
+      <c r="P42" s="116"/>
+      <c r="Q42" s="116"/>
+      <c r="R42" s="116"/>
+      <c r="S42" s="116"/>
+      <c r="T42" s="116"/>
       <c r="U42" s="80"/>
       <c r="V42" s="80"/>
       <c r="W42" s="80"/>
@@ -9790,11 +9790,11 @@
         <f>IF(L44=L31,2,0)</f>
         <v>0</v>
       </c>
-      <c r="M45" s="111" t="str">
+      <c r="M45" s="113" t="str">
         <f>master!G27</f>
         <v>england</v>
       </c>
-      <c r="Q45" s="111" t="str">
+      <c r="Q45" s="113" t="str">
         <f>master!K27</f>
         <v>france</v>
       </c>
@@ -9815,7 +9815,7 @@
       <c r="L46" s="65" t="s">
         <v>234</v>
       </c>
-      <c r="M46" s="112"/>
+      <c r="M46" s="114"/>
       <c r="O46" s="65" t="s">
         <v>151</v>
       </c>
@@ -9962,11 +9962,11 @@
         <f>IF(L50=L37,2,0)</f>
         <v>2</v>
       </c>
-      <c r="M51" s="111" t="str">
+      <c r="M51" s="113" t="str">
         <f>master!G33</f>
         <v>spain</v>
       </c>
-      <c r="Q51" s="111" t="str">
+      <c r="Q51" s="113" t="str">
         <f>master!K33</f>
         <v>usa</v>
       </c>
@@ -9987,7 +9987,7 @@
       <c r="L52" s="65" t="s">
         <v>236</v>
       </c>
-      <c r="M52" s="112"/>
+      <c r="M52" s="114"/>
       <c r="Q52" s="119"/>
       <c r="R52" s="65" t="s">
         <v>240</v>
@@ -10081,6 +10081,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="M51:M52"/>
+    <mergeCell ref="J42:T42"/>
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="M45:M46"/>
+    <mergeCell ref="Q51:Q52"/>
     <mergeCell ref="M32:M33"/>
     <mergeCell ref="Q45:Q46"/>
     <mergeCell ref="B2:G2"/>
@@ -10088,11 +10093,6 @@
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B5:G5"/>
     <mergeCell ref="B6:G6"/>
-    <mergeCell ref="M51:M52"/>
-    <mergeCell ref="J42:T42"/>
-    <mergeCell ref="M38:M39"/>
-    <mergeCell ref="M45:M46"/>
-    <mergeCell ref="Q51:Q52"/>
   </mergeCells>
   <conditionalFormatting sqref="H10 M10 H17 M17 H24 M24">
     <cfRule type="cellIs" dxfId="27" priority="14" operator="equal">
@@ -10175,14 +10175,14 @@
       <c r="A2" s="70">
         <v>5</v>
       </c>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="112" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
       <c r="H2" s="66">
         <v>5</v>
       </c>
@@ -10191,14 +10191,14 @@
       <c r="A3" s="78">
         <v>4</v>
       </c>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="112" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
       <c r="H3" s="66">
         <v>4</v>
       </c>
@@ -10207,14 +10207,14 @@
       <c r="A4" s="73">
         <v>3</v>
       </c>
-      <c r="B4" s="115" t="s">
+      <c r="B4" s="112" t="s">
         <v>143</v>
       </c>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
       <c r="H4" s="66">
         <v>3</v>
       </c>
@@ -10223,14 +10223,14 @@
       <c r="A5" s="79">
         <v>2</v>
       </c>
-      <c r="B5" s="115" t="s">
+      <c r="B5" s="112" t="s">
         <v>144</v>
       </c>
-      <c r="C5" s="115"/>
-      <c r="D5" s="115"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="115"/>
-      <c r="G5" s="115"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
       <c r="H5" s="66">
         <v>2</v>
       </c>
@@ -10239,14 +10239,14 @@
       <c r="A6" s="71">
         <v>1</v>
       </c>
-      <c r="B6" s="115" t="s">
+      <c r="B6" s="112" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="115"/>
-      <c r="D6" s="115"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="115"/>
-      <c r="G6" s="115"/>
+      <c r="C6" s="112"/>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="112"/>
+      <c r="G6" s="112"/>
       <c r="H6" s="66">
         <v>1</v>
       </c>
@@ -11066,19 +11066,19 @@
       <c r="K41" s="64"/>
     </row>
     <row r="42" spans="9:20" x14ac:dyDescent="0.2">
-      <c r="J42" s="114" t="s">
+      <c r="J42" s="116" t="s">
         <v>254</v>
       </c>
-      <c r="K42" s="114"/>
-      <c r="L42" s="114"/>
-      <c r="M42" s="114"/>
-      <c r="N42" s="114"/>
-      <c r="O42" s="114"/>
-      <c r="P42" s="114"/>
-      <c r="Q42" s="114"/>
-      <c r="R42" s="114"/>
-      <c r="S42" s="114"/>
-      <c r="T42" s="114"/>
+      <c r="K42" s="116"/>
+      <c r="L42" s="116"/>
+      <c r="M42" s="116"/>
+      <c r="N42" s="116"/>
+      <c r="O42" s="116"/>
+      <c r="P42" s="116"/>
+      <c r="Q42" s="116"/>
+      <c r="R42" s="116"/>
+      <c r="S42" s="116"/>
+      <c r="T42" s="116"/>
     </row>
     <row r="43" spans="9:20" x14ac:dyDescent="0.2">
       <c r="J43" s="66" t="s">
@@ -11135,11 +11135,11 @@
         <f>IF(L44=L31,2,0)</f>
         <v>2</v>
       </c>
-      <c r="M45" s="111" t="str">
+      <c r="M45" s="113" t="str">
         <f>master!G27</f>
         <v>england</v>
       </c>
-      <c r="Q45" s="111" t="str">
+      <c r="Q45" s="113" t="str">
         <f>master!K27</f>
         <v>france</v>
       </c>
@@ -11160,7 +11160,7 @@
       <c r="L46" s="65" t="s">
         <v>234</v>
       </c>
-      <c r="M46" s="112"/>
+      <c r="M46" s="114"/>
       <c r="O46" s="65" t="s">
         <v>151</v>
       </c>
@@ -11307,11 +11307,11 @@
         <f>IF(L50=L37,2,0)</f>
         <v>0</v>
       </c>
-      <c r="M51" s="111" t="str">
+      <c r="M51" s="113" t="str">
         <f>master!G33</f>
         <v>spain</v>
       </c>
-      <c r="Q51" s="111" t="str">
+      <c r="Q51" s="113" t="str">
         <f>master!K33</f>
         <v>usa</v>
       </c>
@@ -11332,7 +11332,7 @@
       <c r="L52" s="65" t="s">
         <v>236</v>
       </c>
-      <c r="M52" s="112"/>
+      <c r="M52" s="114"/>
       <c r="Q52" s="119"/>
       <c r="R52" s="65" t="s">
         <v>240</v>
@@ -11424,11 +11424,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
     <mergeCell ref="M51:M52"/>
     <mergeCell ref="Q51:Q52"/>
     <mergeCell ref="M32:M33"/>
@@ -11436,6 +11431,11 @@
     <mergeCell ref="J42:T42"/>
     <mergeCell ref="M45:M46"/>
     <mergeCell ref="Q45:Q46"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <conditionalFormatting sqref="H10 N10 H17 N17 H24 N24">
     <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">

</xml_diff>

<commit_message>
re-vamp of how we are seeding teamData
</commit_message>
<xml_diff>
--- a/excel-docs/euro - lifecycle info.xlsx
+++ b/excel-docs/euro - lifecycle info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joseph.collins/Documents/personal-projects/euro/2024_euro/excel-docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2E044C-E03C-0C4F-AD39-C24FCBCF3DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5E38B2-839A-1040-9FB1-5580F50F410B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34560" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D89656BD-B983-D041-A997-C1184058734E}"/>
   </bookViews>
@@ -1510,10 +1510,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1525,6 +1521,10 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2102,8 +2102,8 @@
   </sheetPr>
   <dimension ref="A1:F107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="160" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="160" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2734,14 +2734,14 @@
       <c r="A2" s="70">
         <v>5</v>
       </c>
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="115" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="115"/>
+      <c r="G2" s="115"/>
       <c r="H2" s="66">
         <v>5</v>
       </c>
@@ -2750,14 +2750,14 @@
       <c r="A3" s="78">
         <v>4</v>
       </c>
-      <c r="B3" s="112" t="s">
+      <c r="B3" s="115" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="112"/>
-      <c r="G3" s="112"/>
+      <c r="C3" s="115"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
       <c r="H3" s="66">
         <v>4</v>
       </c>
@@ -2766,14 +2766,14 @@
       <c r="A4" s="73">
         <v>3</v>
       </c>
-      <c r="B4" s="112" t="s">
+      <c r="B4" s="115" t="s">
         <v>143</v>
       </c>
-      <c r="C4" s="112"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
-      <c r="F4" s="112"/>
-      <c r="G4" s="112"/>
+      <c r="C4" s="115"/>
+      <c r="D4" s="115"/>
+      <c r="E4" s="115"/>
+      <c r="F4" s="115"/>
+      <c r="G4" s="115"/>
       <c r="H4" s="66">
         <v>3</v>
       </c>
@@ -2782,14 +2782,14 @@
       <c r="A5" s="79">
         <v>2</v>
       </c>
-      <c r="B5" s="112" t="s">
+      <c r="B5" s="115" t="s">
         <v>144</v>
       </c>
-      <c r="C5" s="112"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
-      <c r="F5" s="112"/>
-      <c r="G5" s="112"/>
+      <c r="C5" s="115"/>
+      <c r="D5" s="115"/>
+      <c r="E5" s="115"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="115"/>
       <c r="H5" s="66">
         <v>2</v>
       </c>
@@ -2798,14 +2798,14 @@
       <c r="A6" s="71">
         <v>1</v>
       </c>
-      <c r="B6" s="112" t="s">
+      <c r="B6" s="115" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="112"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="112"/>
-      <c r="F6" s="112"/>
-      <c r="G6" s="112"/>
+      <c r="C6" s="115"/>
+      <c r="D6" s="115"/>
+      <c r="E6" s="115"/>
+      <c r="F6" s="115"/>
+      <c r="G6" s="115"/>
       <c r="H6" s="66">
         <v>1</v>
       </c>
@@ -3625,19 +3625,19 @@
       <c r="K41" s="64"/>
     </row>
     <row r="42" spans="9:20" x14ac:dyDescent="0.2">
-      <c r="J42" s="116" t="s">
+      <c r="J42" s="114" t="s">
         <v>254</v>
       </c>
-      <c r="K42" s="116"/>
-      <c r="L42" s="116"/>
-      <c r="M42" s="116"/>
-      <c r="N42" s="116"/>
-      <c r="O42" s="116"/>
-      <c r="P42" s="116"/>
-      <c r="Q42" s="116"/>
-      <c r="R42" s="116"/>
-      <c r="S42" s="116"/>
-      <c r="T42" s="116"/>
+      <c r="K42" s="114"/>
+      <c r="L42" s="114"/>
+      <c r="M42" s="114"/>
+      <c r="N42" s="114"/>
+      <c r="O42" s="114"/>
+      <c r="P42" s="114"/>
+      <c r="Q42" s="114"/>
+      <c r="R42" s="114"/>
+      <c r="S42" s="114"/>
+      <c r="T42" s="114"/>
     </row>
     <row r="43" spans="9:20" x14ac:dyDescent="0.2">
       <c r="J43" s="66" t="s">
@@ -3694,11 +3694,11 @@
         <f>IF(L44=L31,2,0)</f>
         <v>0</v>
       </c>
-      <c r="M45" s="113" t="str">
+      <c r="M45" s="111" t="str">
         <f>master!G27</f>
         <v>england</v>
       </c>
-      <c r="Q45" s="113" t="str">
+      <c r="Q45" s="111" t="str">
         <f>master!K27</f>
         <v>france</v>
       </c>
@@ -3719,7 +3719,7 @@
       <c r="L46" s="65" t="s">
         <v>234</v>
       </c>
-      <c r="M46" s="114"/>
+      <c r="M46" s="112"/>
       <c r="O46" s="65" t="s">
         <v>151</v>
       </c>
@@ -3866,11 +3866,11 @@
         <f>IF(L50=L37,2,0)</f>
         <v>2</v>
       </c>
-      <c r="M51" s="113" t="str">
+      <c r="M51" s="111" t="str">
         <f>master!G33</f>
         <v>spain</v>
       </c>
-      <c r="Q51" s="113" t="str">
+      <c r="Q51" s="111" t="str">
         <f>master!K33</f>
         <v>usa</v>
       </c>
@@ -3891,7 +3891,7 @@
       <c r="L52" s="65" t="s">
         <v>236</v>
       </c>
-      <c r="M52" s="114"/>
+      <c r="M52" s="112"/>
       <c r="Q52" s="119"/>
       <c r="R52" s="65" t="s">
         <v>240</v>
@@ -3983,6 +3983,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
     <mergeCell ref="M51:M52"/>
     <mergeCell ref="Q51:Q52"/>
     <mergeCell ref="M32:M33"/>
@@ -3990,11 +3995,6 @@
     <mergeCell ref="J42:T42"/>
     <mergeCell ref="M45:M46"/>
     <mergeCell ref="Q45:Q46"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <conditionalFormatting sqref="H10 N10 H17 N17 H24 N24">
     <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
@@ -4077,14 +4077,14 @@
       <c r="A2" s="70">
         <v>5</v>
       </c>
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="115" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="115"/>
+      <c r="G2" s="115"/>
       <c r="H2" s="66">
         <v>5</v>
       </c>
@@ -4093,14 +4093,14 @@
       <c r="A3" s="78">
         <v>4</v>
       </c>
-      <c r="B3" s="112" t="s">
+      <c r="B3" s="115" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="112"/>
-      <c r="G3" s="112"/>
+      <c r="C3" s="115"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
       <c r="H3" s="66">
         <v>4</v>
       </c>
@@ -4109,14 +4109,14 @@
       <c r="A4" s="73">
         <v>3</v>
       </c>
-      <c r="B4" s="112" t="s">
+      <c r="B4" s="115" t="s">
         <v>143</v>
       </c>
-      <c r="C4" s="112"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
-      <c r="F4" s="112"/>
-      <c r="G4" s="112"/>
+      <c r="C4" s="115"/>
+      <c r="D4" s="115"/>
+      <c r="E4" s="115"/>
+      <c r="F4" s="115"/>
+      <c r="G4" s="115"/>
       <c r="H4" s="66">
         <v>3</v>
       </c>
@@ -4125,14 +4125,14 @@
       <c r="A5" s="79">
         <v>2</v>
       </c>
-      <c r="B5" s="112" t="s">
+      <c r="B5" s="115" t="s">
         <v>144</v>
       </c>
-      <c r="C5" s="112"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
-      <c r="F5" s="112"/>
-      <c r="G5" s="112"/>
+      <c r="C5" s="115"/>
+      <c r="D5" s="115"/>
+      <c r="E5" s="115"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="115"/>
       <c r="H5" s="66">
         <v>2</v>
       </c>
@@ -4141,14 +4141,14 @@
       <c r="A6" s="71">
         <v>1</v>
       </c>
-      <c r="B6" s="112" t="s">
+      <c r="B6" s="115" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="112"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="112"/>
-      <c r="F6" s="112"/>
-      <c r="G6" s="112"/>
+      <c r="C6" s="115"/>
+      <c r="D6" s="115"/>
+      <c r="E6" s="115"/>
+      <c r="F6" s="115"/>
+      <c r="G6" s="115"/>
       <c r="H6" s="66">
         <v>1</v>
       </c>
@@ -4968,19 +4968,19 @@
       <c r="K41" s="64"/>
     </row>
     <row r="42" spans="9:20" x14ac:dyDescent="0.2">
-      <c r="J42" s="116" t="s">
+      <c r="J42" s="114" t="s">
         <v>254</v>
       </c>
-      <c r="K42" s="116"/>
-      <c r="L42" s="116"/>
-      <c r="M42" s="116"/>
-      <c r="N42" s="116"/>
-      <c r="O42" s="116"/>
-      <c r="P42" s="116"/>
-      <c r="Q42" s="116"/>
-      <c r="R42" s="116"/>
-      <c r="S42" s="116"/>
-      <c r="T42" s="116"/>
+      <c r="K42" s="114"/>
+      <c r="L42" s="114"/>
+      <c r="M42" s="114"/>
+      <c r="N42" s="114"/>
+      <c r="O42" s="114"/>
+      <c r="P42" s="114"/>
+      <c r="Q42" s="114"/>
+      <c r="R42" s="114"/>
+      <c r="S42" s="114"/>
+      <c r="T42" s="114"/>
     </row>
     <row r="43" spans="9:20" x14ac:dyDescent="0.2">
       <c r="J43" s="66" t="s">
@@ -5037,11 +5037,11 @@
         <f>IF(L44=L31,2,0)</f>
         <v>2</v>
       </c>
-      <c r="M45" s="113" t="str">
+      <c r="M45" s="111" t="str">
         <f>master!G27</f>
         <v>england</v>
       </c>
-      <c r="Q45" s="113" t="str">
+      <c r="Q45" s="111" t="str">
         <f>master!K27</f>
         <v>france</v>
       </c>
@@ -5062,7 +5062,7 @@
       <c r="L46" s="65" t="s">
         <v>234</v>
       </c>
-      <c r="M46" s="114"/>
+      <c r="M46" s="112"/>
       <c r="O46" s="65" t="s">
         <v>151</v>
       </c>
@@ -5209,11 +5209,11 @@
         <f>IF(L50=L37,2,0)</f>
         <v>0</v>
       </c>
-      <c r="M51" s="113" t="str">
+      <c r="M51" s="111" t="str">
         <f>master!G33</f>
         <v>spain</v>
       </c>
-      <c r="Q51" s="113" t="str">
+      <c r="Q51" s="111" t="str">
         <f>master!K33</f>
         <v>usa</v>
       </c>
@@ -5234,7 +5234,7 @@
       <c r="L52" s="65" t="s">
         <v>236</v>
       </c>
-      <c r="M52" s="114"/>
+      <c r="M52" s="112"/>
       <c r="Q52" s="119"/>
       <c r="R52" s="65" t="s">
         <v>240</v>
@@ -5326,6 +5326,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
     <mergeCell ref="M51:M52"/>
     <mergeCell ref="Q51:Q52"/>
     <mergeCell ref="M32:M33"/>
@@ -5333,11 +5338,6 @@
     <mergeCell ref="J42:T42"/>
     <mergeCell ref="M45:M46"/>
     <mergeCell ref="Q45:Q46"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <conditionalFormatting sqref="H10 N10 H17 N17 H24 N24">
     <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
@@ -5409,15 +5409,15 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="116" t="s">
+      <c r="A2" s="114" t="s">
         <v>228</v>
       </c>
-      <c r="B2" s="116"/>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
+      <c r="B2" s="114"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="114"/>
+      <c r="G2" s="114"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="122" t="s">
@@ -5593,15 +5593,15 @@
       <c r="G13" s="121"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="116" t="s">
+      <c r="A16" s="114" t="s">
         <v>241</v>
       </c>
-      <c r="B16" s="116"/>
-      <c r="C16" s="116"/>
-      <c r="D16" s="116"/>
-      <c r="E16" s="116"/>
-      <c r="F16" s="116"/>
-      <c r="G16" s="116"/>
+      <c r="B16" s="114"/>
+      <c r="C16" s="114"/>
+      <c r="D16" s="114"/>
+      <c r="E16" s="114"/>
+      <c r="F16" s="114"/>
+      <c r="G16" s="114"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="120" t="s">
@@ -5778,6 +5778,9 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A20:A21"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="G3:G4"/>
@@ -5793,9 +5796,6 @@
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A20:A21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7074,14 +7074,14 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="68"/>
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="115" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="115"/>
+      <c r="G2" s="115"/>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
@@ -7092,14 +7092,14 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="77"/>
-      <c r="B3" s="112" t="s">
+      <c r="B3" s="115" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="112"/>
-      <c r="G3" s="112"/>
+      <c r="C3" s="115"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
@@ -7110,14 +7110,14 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="72"/>
-      <c r="B4" s="112" t="s">
+      <c r="B4" s="115" t="s">
         <v>143</v>
       </c>
-      <c r="C4" s="112"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
-      <c r="F4" s="112"/>
-      <c r="G4" s="112"/>
+      <c r="C4" s="115"/>
+      <c r="D4" s="115"/>
+      <c r="E4" s="115"/>
+      <c r="F4" s="115"/>
+      <c r="G4" s="115"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
@@ -7128,14 +7128,14 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="69"/>
-      <c r="B5" s="112" t="s">
+      <c r="B5" s="115" t="s">
         <v>144</v>
       </c>
-      <c r="C5" s="112"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
-      <c r="F5" s="112"/>
-      <c r="G5" s="112"/>
+      <c r="C5" s="115"/>
+      <c r="D5" s="115"/>
+      <c r="E5" s="115"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="115"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
@@ -7146,14 +7146,14 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="22"/>
-      <c r="B6" s="112" t="s">
+      <c r="B6" s="115" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="112"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="112"/>
-      <c r="F6" s="112"/>
-      <c r="G6" s="112"/>
+      <c r="C6" s="115"/>
+      <c r="D6" s="115"/>
+      <c r="E6" s="115"/>
+      <c r="F6" s="115"/>
+      <c r="G6" s="115"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
@@ -8064,7 +8064,7 @@
       <c r="AE30" s="89"/>
     </row>
     <row r="31" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C31" s="111"/>
+      <c r="C31" s="116"/>
       <c r="D31" s="66" t="s">
         <v>210</v>
       </c>
@@ -8086,7 +8086,7 @@
       </c>
     </row>
     <row r="32" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C32" s="111"/>
+      <c r="C32" s="116"/>
       <c r="D32" s="76" t="s">
         <v>220</v>
       </c>
@@ -8131,7 +8131,7 @@
       <c r="AE33" s="89"/>
     </row>
     <row r="34" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C34" s="111"/>
+      <c r="C34" s="116"/>
       <c r="D34" s="70" t="s">
         <v>211</v>
       </c>
@@ -8158,7 +8158,7 @@
       </c>
     </row>
     <row r="35" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C35" s="111"/>
+      <c r="C35" s="116"/>
       <c r="D35" s="70" t="s">
         <v>216</v>
       </c>
@@ -8205,7 +8205,7 @@
       <c r="AE36" s="89"/>
     </row>
     <row r="37" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C37" s="111"/>
+      <c r="C37" s="116"/>
       <c r="D37" s="66" t="s">
         <v>224</v>
       </c>
@@ -8228,7 +8228,7 @@
       </c>
     </row>
     <row r="38" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C38" s="111"/>
+      <c r="C38" s="116"/>
       <c r="D38" s="76" t="s">
         <v>255</v>
       </c>
@@ -8253,7 +8253,7 @@
       <c r="X38" s="76" t="s">
         <v>226</v>
       </c>
-      <c r="AE38" s="111"/>
+      <c r="AE38" s="116"/>
     </row>
     <row r="39" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C39"/>
@@ -8267,10 +8267,10 @@
       </c>
       <c r="W39" s="66"/>
       <c r="X39" s="66"/>
-      <c r="AE39" s="111"/>
+      <c r="AE39" s="116"/>
     </row>
     <row r="40" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C40" s="111"/>
+      <c r="C40" s="116"/>
       <c r="D40" s="70" t="s">
         <v>219</v>
       </c>
@@ -8293,7 +8293,7 @@
       </c>
     </row>
     <row r="41" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C41" s="111"/>
+      <c r="C41" s="116"/>
       <c r="D41" s="70" t="s">
         <v>222</v>
       </c>
@@ -8314,29 +8314,29 @@
       </c>
     </row>
     <row r="43" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="D43" s="116" t="s">
+      <c r="D43" s="114" t="s">
         <v>254</v>
       </c>
-      <c r="E43" s="116"/>
-      <c r="F43" s="116"/>
-      <c r="G43" s="116"/>
-      <c r="H43" s="116"/>
-      <c r="I43" s="116"/>
-      <c r="J43" s="116"/>
-      <c r="K43" s="116"/>
-      <c r="L43" s="116"/>
-      <c r="M43" s="116"/>
-      <c r="N43" s="116"/>
-      <c r="O43" s="116"/>
-      <c r="P43" s="116"/>
-      <c r="Q43" s="116"/>
-      <c r="R43" s="116"/>
-      <c r="S43" s="116"/>
-      <c r="T43" s="116"/>
-      <c r="U43" s="116"/>
-      <c r="V43" s="116"/>
-      <c r="W43" s="116"/>
-      <c r="X43" s="116"/>
+      <c r="E43" s="114"/>
+      <c r="F43" s="114"/>
+      <c r="G43" s="114"/>
+      <c r="H43" s="114"/>
+      <c r="I43" s="114"/>
+      <c r="J43" s="114"/>
+      <c r="K43" s="114"/>
+      <c r="L43" s="114"/>
+      <c r="M43" s="114"/>
+      <c r="N43" s="114"/>
+      <c r="O43" s="114"/>
+      <c r="P43" s="114"/>
+      <c r="Q43" s="114"/>
+      <c r="R43" s="114"/>
+      <c r="S43" s="114"/>
+      <c r="T43" s="114"/>
+      <c r="U43" s="114"/>
+      <c r="V43" s="114"/>
+      <c r="W43" s="114"/>
+      <c r="X43" s="114"/>
     </row>
     <row r="44" spans="3:31" x14ac:dyDescent="0.2">
       <c r="D44" s="66" t="s">
@@ -8395,12 +8395,12 @@
         <f>IF(F45=F32,2,0)</f>
         <v>2</v>
       </c>
-      <c r="G46" s="113" t="str">
+      <c r="G46" s="111" t="str">
         <f>master!G27</f>
         <v>england</v>
       </c>
       <c r="M46" s="64"/>
-      <c r="P46" s="115" t="str">
+      <c r="P46" s="113" t="str">
         <f>master!K27</f>
         <v>france</v>
       </c>
@@ -8421,12 +8421,12 @@
       <c r="F47" s="65" t="s">
         <v>234</v>
       </c>
-      <c r="G47" s="114"/>
+      <c r="G47" s="112"/>
       <c r="M47" s="67"/>
       <c r="N47" s="65" t="s">
         <v>151</v>
       </c>
-      <c r="P47" s="115"/>
+      <c r="P47" s="113"/>
       <c r="V47" s="90" t="s">
         <v>238</v>
       </c>
@@ -8455,7 +8455,7 @@
       <c r="L48" s="65" t="s">
         <v>224</v>
       </c>
-      <c r="N48" s="115" t="str">
+      <c r="N48" s="113" t="str">
         <f>master!I29</f>
         <v>france</v>
       </c>
@@ -8484,12 +8484,12 @@
         <f>IF(F48=F35,2,0)</f>
         <v>2</v>
       </c>
-      <c r="L49" s="115" t="str">
+      <c r="L49" s="113" t="str">
         <f>master!H30</f>
         <v>england</v>
       </c>
-      <c r="N49" s="115"/>
-      <c r="O49" s="115" t="str">
+      <c r="N49" s="113"/>
+      <c r="O49" s="113" t="str">
         <f>master!J30</f>
         <v>france</v>
       </c>
@@ -8510,12 +8510,12 @@
       <c r="F50" s="65" t="s">
         <v>235</v>
       </c>
-      <c r="L50" s="115"/>
+      <c r="L50" s="113"/>
       <c r="N50" s="64">
         <f>IF(N48=N35,10,0)</f>
         <v>10</v>
       </c>
-      <c r="O50" s="115"/>
+      <c r="O50" s="113"/>
       <c r="V50" s="65" t="s">
         <v>239</v>
       </c>
@@ -8568,11 +8568,11 @@
         <f>IF(F51=F38,2,0)</f>
         <v>2</v>
       </c>
-      <c r="G52" s="113" t="str">
+      <c r="G52" s="111" t="str">
         <f>master!G33</f>
         <v>spain</v>
       </c>
-      <c r="P52" s="115" t="str">
+      <c r="P52" s="113" t="str">
         <f>master!K33</f>
         <v>usa</v>
       </c>
@@ -8593,8 +8593,8 @@
       <c r="F53" s="65" t="s">
         <v>236</v>
       </c>
-      <c r="G53" s="114"/>
-      <c r="P53" s="115"/>
+      <c r="G53" s="112"/>
+      <c r="P53" s="113"/>
       <c r="V53" s="65" t="s">
         <v>240</v>
       </c>
@@ -8714,19 +8714,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="P52:P53"/>
-    <mergeCell ref="D43:X43"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="P46:P47"/>
-    <mergeCell ref="N48:N49"/>
-    <mergeCell ref="L49:L50"/>
-    <mergeCell ref="O49:O50"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="AE38:AE39"/>
     <mergeCell ref="G39:G40"/>
@@ -8739,6 +8726,19 @@
     <mergeCell ref="L36:L37"/>
     <mergeCell ref="O36:O37"/>
     <mergeCell ref="N35:N36"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="P52:P53"/>
+    <mergeCell ref="D43:X43"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="P46:P47"/>
+    <mergeCell ref="N48:N49"/>
+    <mergeCell ref="L49:L50"/>
+    <mergeCell ref="O49:O50"/>
   </mergeCells>
   <conditionalFormatting sqref="L10 V10 L17 V17 L24 V24">
     <cfRule type="cellIs" dxfId="32" priority="6" operator="equal">
@@ -8800,14 +8800,14 @@
       <c r="A2" s="70">
         <v>5</v>
       </c>
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="115" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="115"/>
+      <c r="G2" s="115"/>
       <c r="H2" s="66">
         <v>5</v>
       </c>
@@ -8816,14 +8816,14 @@
       <c r="A3" s="78">
         <v>4</v>
       </c>
-      <c r="B3" s="112" t="s">
+      <c r="B3" s="115" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="112"/>
-      <c r="G3" s="112"/>
+      <c r="C3" s="115"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
       <c r="H3" s="66">
         <v>4</v>
       </c>
@@ -8832,14 +8832,14 @@
       <c r="A4" s="73">
         <v>3</v>
       </c>
-      <c r="B4" s="112" t="s">
+      <c r="B4" s="115" t="s">
         <v>143</v>
       </c>
-      <c r="C4" s="112"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
-      <c r="F4" s="112"/>
-      <c r="G4" s="112"/>
+      <c r="C4" s="115"/>
+      <c r="D4" s="115"/>
+      <c r="E4" s="115"/>
+      <c r="F4" s="115"/>
+      <c r="G4" s="115"/>
       <c r="H4" s="66">
         <v>3</v>
       </c>
@@ -8848,14 +8848,14 @@
       <c r="A5" s="79">
         <v>2</v>
       </c>
-      <c r="B5" s="112" t="s">
+      <c r="B5" s="115" t="s">
         <v>144</v>
       </c>
-      <c r="C5" s="112"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
-      <c r="F5" s="112"/>
-      <c r="G5" s="112"/>
+      <c r="C5" s="115"/>
+      <c r="D5" s="115"/>
+      <c r="E5" s="115"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="115"/>
       <c r="H5" s="66">
         <v>2</v>
       </c>
@@ -8864,14 +8864,14 @@
       <c r="A6" s="71">
         <v>1</v>
       </c>
-      <c r="B6" s="112" t="s">
+      <c r="B6" s="115" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="112"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="112"/>
-      <c r="F6" s="112"/>
-      <c r="G6" s="112"/>
+      <c r="C6" s="115"/>
+      <c r="D6" s="115"/>
+      <c r="E6" s="115"/>
+      <c r="F6" s="115"/>
+      <c r="G6" s="115"/>
       <c r="H6" s="66">
         <v>1</v>
       </c>
@@ -9711,19 +9711,19 @@
       <c r="K41" s="64"/>
     </row>
     <row r="42" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="J42" s="116" t="s">
+      <c r="J42" s="114" t="s">
         <v>254</v>
       </c>
-      <c r="K42" s="116"/>
-      <c r="L42" s="116"/>
-      <c r="M42" s="116"/>
-      <c r="N42" s="116"/>
-      <c r="O42" s="116"/>
-      <c r="P42" s="116"/>
-      <c r="Q42" s="116"/>
-      <c r="R42" s="116"/>
-      <c r="S42" s="116"/>
-      <c r="T42" s="116"/>
+      <c r="K42" s="114"/>
+      <c r="L42" s="114"/>
+      <c r="M42" s="114"/>
+      <c r="N42" s="114"/>
+      <c r="O42" s="114"/>
+      <c r="P42" s="114"/>
+      <c r="Q42" s="114"/>
+      <c r="R42" s="114"/>
+      <c r="S42" s="114"/>
+      <c r="T42" s="114"/>
       <c r="U42" s="80"/>
       <c r="V42" s="80"/>
       <c r="W42" s="80"/>
@@ -9790,11 +9790,11 @@
         <f>IF(L44=L31,2,0)</f>
         <v>0</v>
       </c>
-      <c r="M45" s="113" t="str">
+      <c r="M45" s="111" t="str">
         <f>master!G27</f>
         <v>england</v>
       </c>
-      <c r="Q45" s="113" t="str">
+      <c r="Q45" s="111" t="str">
         <f>master!K27</f>
         <v>france</v>
       </c>
@@ -9815,7 +9815,7 @@
       <c r="L46" s="65" t="s">
         <v>234</v>
       </c>
-      <c r="M46" s="114"/>
+      <c r="M46" s="112"/>
       <c r="O46" s="65" t="s">
         <v>151</v>
       </c>
@@ -9962,11 +9962,11 @@
         <f>IF(L50=L37,2,0)</f>
         <v>2</v>
       </c>
-      <c r="M51" s="113" t="str">
+      <c r="M51" s="111" t="str">
         <f>master!G33</f>
         <v>spain</v>
       </c>
-      <c r="Q51" s="113" t="str">
+      <c r="Q51" s="111" t="str">
         <f>master!K33</f>
         <v>usa</v>
       </c>
@@ -9987,7 +9987,7 @@
       <c r="L52" s="65" t="s">
         <v>236</v>
       </c>
-      <c r="M52" s="114"/>
+      <c r="M52" s="112"/>
       <c r="Q52" s="119"/>
       <c r="R52" s="65" t="s">
         <v>240</v>
@@ -10081,11 +10081,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="M51:M52"/>
-    <mergeCell ref="J42:T42"/>
-    <mergeCell ref="M38:M39"/>
-    <mergeCell ref="M45:M46"/>
-    <mergeCell ref="Q51:Q52"/>
     <mergeCell ref="M32:M33"/>
     <mergeCell ref="Q45:Q46"/>
     <mergeCell ref="B2:G2"/>
@@ -10093,6 +10088,11 @@
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B5:G5"/>
     <mergeCell ref="B6:G6"/>
+    <mergeCell ref="M51:M52"/>
+    <mergeCell ref="J42:T42"/>
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="M45:M46"/>
+    <mergeCell ref="Q51:Q52"/>
   </mergeCells>
   <conditionalFormatting sqref="H10 M10 H17 M17 H24 M24">
     <cfRule type="cellIs" dxfId="27" priority="14" operator="equal">
@@ -10175,14 +10175,14 @@
       <c r="A2" s="70">
         <v>5</v>
       </c>
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="115" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="115"/>
+      <c r="G2" s="115"/>
       <c r="H2" s="66">
         <v>5</v>
       </c>
@@ -10191,14 +10191,14 @@
       <c r="A3" s="78">
         <v>4</v>
       </c>
-      <c r="B3" s="112" t="s">
+      <c r="B3" s="115" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="112"/>
-      <c r="G3" s="112"/>
+      <c r="C3" s="115"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
       <c r="H3" s="66">
         <v>4</v>
       </c>
@@ -10207,14 +10207,14 @@
       <c r="A4" s="73">
         <v>3</v>
       </c>
-      <c r="B4" s="112" t="s">
+      <c r="B4" s="115" t="s">
         <v>143</v>
       </c>
-      <c r="C4" s="112"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
-      <c r="F4" s="112"/>
-      <c r="G4" s="112"/>
+      <c r="C4" s="115"/>
+      <c r="D4" s="115"/>
+      <c r="E4" s="115"/>
+      <c r="F4" s="115"/>
+      <c r="G4" s="115"/>
       <c r="H4" s="66">
         <v>3</v>
       </c>
@@ -10223,14 +10223,14 @@
       <c r="A5" s="79">
         <v>2</v>
       </c>
-      <c r="B5" s="112" t="s">
+      <c r="B5" s="115" t="s">
         <v>144</v>
       </c>
-      <c r="C5" s="112"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
-      <c r="F5" s="112"/>
-      <c r="G5" s="112"/>
+      <c r="C5" s="115"/>
+      <c r="D5" s="115"/>
+      <c r="E5" s="115"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="115"/>
       <c r="H5" s="66">
         <v>2</v>
       </c>
@@ -10239,14 +10239,14 @@
       <c r="A6" s="71">
         <v>1</v>
       </c>
-      <c r="B6" s="112" t="s">
+      <c r="B6" s="115" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="112"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="112"/>
-      <c r="F6" s="112"/>
-      <c r="G6" s="112"/>
+      <c r="C6" s="115"/>
+      <c r="D6" s="115"/>
+      <c r="E6" s="115"/>
+      <c r="F6" s="115"/>
+      <c r="G6" s="115"/>
       <c r="H6" s="66">
         <v>1</v>
       </c>
@@ -11066,19 +11066,19 @@
       <c r="K41" s="64"/>
     </row>
     <row r="42" spans="9:20" x14ac:dyDescent="0.2">
-      <c r="J42" s="116" t="s">
+      <c r="J42" s="114" t="s">
         <v>254</v>
       </c>
-      <c r="K42" s="116"/>
-      <c r="L42" s="116"/>
-      <c r="M42" s="116"/>
-      <c r="N42" s="116"/>
-      <c r="O42" s="116"/>
-      <c r="P42" s="116"/>
-      <c r="Q42" s="116"/>
-      <c r="R42" s="116"/>
-      <c r="S42" s="116"/>
-      <c r="T42" s="116"/>
+      <c r="K42" s="114"/>
+      <c r="L42" s="114"/>
+      <c r="M42" s="114"/>
+      <c r="N42" s="114"/>
+      <c r="O42" s="114"/>
+      <c r="P42" s="114"/>
+      <c r="Q42" s="114"/>
+      <c r="R42" s="114"/>
+      <c r="S42" s="114"/>
+      <c r="T42" s="114"/>
     </row>
     <row r="43" spans="9:20" x14ac:dyDescent="0.2">
       <c r="J43" s="66" t="s">
@@ -11135,11 +11135,11 @@
         <f>IF(L44=L31,2,0)</f>
         <v>2</v>
       </c>
-      <c r="M45" s="113" t="str">
+      <c r="M45" s="111" t="str">
         <f>master!G27</f>
         <v>england</v>
       </c>
-      <c r="Q45" s="113" t="str">
+      <c r="Q45" s="111" t="str">
         <f>master!K27</f>
         <v>france</v>
       </c>
@@ -11160,7 +11160,7 @@
       <c r="L46" s="65" t="s">
         <v>234</v>
       </c>
-      <c r="M46" s="114"/>
+      <c r="M46" s="112"/>
       <c r="O46" s="65" t="s">
         <v>151</v>
       </c>
@@ -11307,11 +11307,11 @@
         <f>IF(L50=L37,2,0)</f>
         <v>0</v>
       </c>
-      <c r="M51" s="113" t="str">
+      <c r="M51" s="111" t="str">
         <f>master!G33</f>
         <v>spain</v>
       </c>
-      <c r="Q51" s="113" t="str">
+      <c r="Q51" s="111" t="str">
         <f>master!K33</f>
         <v>usa</v>
       </c>
@@ -11332,7 +11332,7 @@
       <c r="L52" s="65" t="s">
         <v>236</v>
       </c>
-      <c r="M52" s="114"/>
+      <c r="M52" s="112"/>
       <c r="Q52" s="119"/>
       <c r="R52" s="65" t="s">
         <v>240</v>
@@ -11424,6 +11424,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
     <mergeCell ref="M51:M52"/>
     <mergeCell ref="Q51:Q52"/>
     <mergeCell ref="M32:M33"/>
@@ -11431,11 +11436,6 @@
     <mergeCell ref="J42:T42"/>
     <mergeCell ref="M45:M46"/>
     <mergeCell ref="Q45:Q46"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <conditionalFormatting sqref="H10 N10 H17 N17 H24 N24">
     <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">

</xml_diff>